<commit_message>
Actualización automática 2025-05-22 17:10:06
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3461,7 +3461,7 @@
         <v>5689.68</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>13971.48</v>
+        <v>18337.68</v>
       </c>
     </row>
     <row r="11">
@@ -3917,7 +3917,7 @@
         <v>114.19</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>384.05</v>
+        <v>787.97</v>
       </c>
     </row>
     <row r="30">
@@ -4555,7 +4555,7 @@
         <v>31281.76</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>32583.96</v>
+        <v>37354.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-26 13:00:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3869,7 +3869,7 @@
         <v>370.41</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>3871.06</v>
+        <v>3865.18</v>
       </c>
     </row>
     <row r="28">
@@ -4555,7 +4555,7 @@
         <v>31281.76</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>37354.08</v>
+        <v>37348.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-26 13:20:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3461,7 +3461,7 @@
         <v>5689.68</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>18337.68</v>
+        <v>18249.33</v>
       </c>
     </row>
     <row r="11">
@@ -4555,7 +4555,7 @@
         <v>31281.76</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>37348.2</v>
+        <v>37259.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-27 17:00:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -4349,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>3375.89</v>
+        <v>3470.45</v>
       </c>
     </row>
     <row r="48">
@@ -4541,7 +4541,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0</v>
+        <v>808.39</v>
       </c>
     </row>
     <row r="56">
@@ -4555,7 +4555,7 @@
         <v>31281.76</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>37259.85</v>
+        <v>38162.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-28 11:25:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>1605.8</v>
+        <v>1623.81</v>
       </c>
     </row>
     <row r="27">
@@ -4555,7 +4555,7 @@
         <v>31281.76</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>38162.8</v>
+        <v>38180.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-30 17:55:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -622,13 +622,13 @@
         <v>0</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>-10.76</v>
+        <v>1765.1</v>
       </c>
       <c r="M3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0</v>
+        <v>1551.05</v>
       </c>
     </row>
     <row r="4">
@@ -3175,7 +3175,7 @@
       </c>
       <c r="L56" s="4" t="inlineStr">
         <is>
-          <t>9 de 54</t>
+          <t>10 de 54</t>
         </is>
       </c>
       <c r="M56" s="4" t="inlineStr">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="N56" s="4" t="inlineStr">
         <is>
-          <t>2 de 54</t>
+          <t>3 de 54</t>
         </is>
       </c>
     </row>
@@ -3293,7 +3293,7 @@
         <v>2478.81</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>-10.76</v>
+        <v>3316.15</v>
       </c>
     </row>
     <row r="4">
@@ -4555,7 +4555,7 @@
         <v>31281.76</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>47031.99</v>
+        <v>50358.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-03 17:25:06
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1774,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>0</v>
+        <v>133.06</v>
       </c>
       <c r="M27" s="2" t="n">
         <v>0</v>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="L56" s="4" t="inlineStr">
         <is>
-          <t>0 de 54</t>
+          <t>1 de 54</t>
         </is>
       </c>
       <c r="M56" s="4" t="inlineStr">
@@ -3213,7 +3213,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -3950,7 +3950,7 @@
         <v>3865.18</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0</v>
+        <v>133.06</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>0</v>
@@ -4723,7 +4723,7 @@
         <v>50358.9</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>0</v>
+        <v>133.06</v>
       </c>
       <c r="G56" s="6" t="n">
         <v>50500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-06-04 15:00:06
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2782,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="2" t="n">
-        <v>0</v>
+        <v>75.31999999999999</v>
       </c>
       <c r="M48" s="2" t="n">
         <v>0</v>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="L56" s="4" t="inlineStr">
         <is>
-          <t>1 de 54</t>
+          <t>2 de 54</t>
         </is>
       </c>
       <c r="M56" s="4" t="inlineStr">
@@ -4517,7 +4517,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>0</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>1000</v>
@@ -4723,7 +4723,7 @@
         <v>50358.9</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>133.06</v>
+        <v>217.96</v>
       </c>
       <c r="G56" s="6" t="n">
         <v>50500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-06-04 15:05:06
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3022,7 +3022,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M53" s="2" t="n">
         <v>0</v>
@@ -3175,7 +3175,7 @@
       </c>
       <c r="L56" s="4" t="inlineStr">
         <is>
-          <t>2 de 54</t>
+          <t>3 de 54</t>
         </is>
       </c>
       <c r="M56" s="4" t="inlineStr">
@@ -4652,7 +4652,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>500</v>
@@ -4723,7 +4723,7 @@
         <v>50358.9</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>217.96</v>
+        <v>242.96</v>
       </c>
       <c r="G56" s="6" t="n">
         <v>50500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-06-09 12:40:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2498,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="2" t="n">
-        <v>-18.25</v>
+        <v>-59.72</v>
       </c>
       <c r="M42" s="2" t="n">
         <v>0</v>
@@ -4359,7 +4359,7 @@
         <v>1167.85</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>-18.25</v>
+        <v>-59.72</v>
       </c>
       <c r="G42" s="2" t="n">
         <v>2000</v>
@@ -4727,7 +4727,7 @@
         <v>50358.9</v>
       </c>
       <c r="F56" s="6" t="n">
-        <v>224.71</v>
+        <v>183.24</v>
       </c>
       <c r="G56" s="6" t="n">
         <v>50500</v>
@@ -4756,8 +4756,8 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5143,13 +5143,13 @@
         <v>38417.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>215.13</v>
+        <v>173.66</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>38202.04</v>
+        <v>38243.50999999999</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.00559983986326947</v>
+        <v>0.004520374613746926</v>
       </c>
     </row>
     <row r="17">
@@ -5210,13 +5210,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>224.71</v>
+        <v>183.24</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>55184.99560036208</v>
+        <v>55226.46560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.004055426708466967</v>
+        <v>0.003307001869340426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-09 15:40:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
+          <t>IMPORTADORA ORTEGA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
+          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2035,7 +2035,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LUI WONG ANGEL BOLIVAR</t>
+          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MENA COSTA GUIDO LENNIN</t>
+          <t>LUI WONG ANGEL BOLIVAR</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MINUTOCORP S.A.</t>
+          <t>MENA COSTA GUIDO LENNIN</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
+          <t>MINUTOCORP S.A.</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MORALES GRACIELA ENITH</t>
+          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
+          <t>MORALES GRACIELA ENITH</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
+          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2419,7 +2419,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -2498,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="2" t="n">
-        <v>-59.72</v>
+        <v>0</v>
       </c>
       <c r="M42" s="2" t="n">
         <v>0</v>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="2" t="n">
-        <v>0</v>
+        <v>-59.72</v>
       </c>
       <c r="M43" s="2" t="n">
         <v>0</v>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="L48" s="2" t="n">
-        <v>75.31999999999999</v>
+        <v>0</v>
       </c>
       <c r="M48" s="2" t="n">
         <v>0</v>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="2" t="n">
-        <v>0</v>
+        <v>75.31999999999999</v>
       </c>
       <c r="M49" s="2" t="n">
         <v>0</v>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
@@ -2899,7 +2899,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -3026,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="L53" s="2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M53" s="2" t="n">
         <v>0</v>
@@ -3043,7 +3043,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -3074,7 +3074,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M54" s="2" t="n">
         <v>0</v>
@@ -3091,105 +3091,153 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="C56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="D56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="E56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="F56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="G56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="H56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="I56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="J56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="K56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="L56" s="4" t="inlineStr">
-        <is>
-          <t>3 de 54</t>
-        </is>
-      </c>
-      <c r="M56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
-        </is>
-      </c>
-      <c r="N56" s="4" t="inlineStr">
-        <is>
-          <t>0 de 54</t>
+      <c r="C56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="D57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="E57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="F57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="H57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="I57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="J57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="K57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="L57" s="4" t="inlineStr">
+        <is>
+          <t>3 de 55</t>
+        </is>
+      </c>
+      <c r="M57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
+        </is>
+      </c>
+      <c r="N57" s="4" t="inlineStr">
+        <is>
+          <t>0 de 55</t>
         </is>
       </c>
     </row>
@@ -3204,7 +3252,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4049,7 +4097,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
+          <t>IMPORTADORA ORTEGA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -4065,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -4076,7 +4124,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
+          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -4092,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="33">
@@ -4103,7 +4151,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LUI WONG ANGEL BOLIVAR</t>
+          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -4130,7 +4178,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>MENA COSTA GUIDO LENNIN</t>
+          <t>LUI WONG ANGEL BOLIVAR</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -4157,7 +4205,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MINUTOCORP S.A.</t>
+          <t>MENA COSTA GUIDO LENNIN</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -4184,7 +4232,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
+          <t>MINUTOCORP S.A.</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -4200,7 +4248,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="2" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -4211,7 +4259,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MORALES GRACIELA ENITH</t>
+          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -4238,11 +4286,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
+          <t>MORALES GRACIELA ENITH</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>1875.17</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="n">
         <v>0</v>
@@ -4254,7 +4302,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="2" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="39">
@@ -4265,11 +4313,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
+          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>0</v>
+        <v>1875.17</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>0</v>
@@ -4281,7 +4329,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="40">
@@ -4292,7 +4340,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -4319,7 +4367,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -4346,23 +4394,23 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>2078.33</v>
+        <v>0</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>3838.11</v>
+        <v>0</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>1167.85</v>
+        <v>0</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>-59.72</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -4373,23 +4421,23 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>1278.13</v>
+        <v>2078.33</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>1912.87</v>
+        <v>3838.11</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>737.72</v>
+        <v>1167.85</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>0</v>
+        <v>-59.72</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="44">
@@ -4400,23 +4448,23 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>0</v>
+        <v>1278.13</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0</v>
+        <v>1912.87</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>0</v>
+        <v>737.72</v>
       </c>
       <c r="F44" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="45">
@@ -4427,7 +4475,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -4454,17 +4502,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>131.6</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>1709.57</v>
+        <v>0</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>598.58</v>
+        <v>0</v>
       </c>
       <c r="F46" s="2" t="n">
         <v>0</v>
@@ -4481,23 +4529,23 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>0</v>
+        <v>131.6</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>0</v>
+        <v>1709.57</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>3470.45</v>
+        <v>598.58</v>
       </c>
       <c r="F47" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -4508,20 +4556,20 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>68.04000000000001</v>
+        <v>0</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>0</v>
+        <v>3470.45</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>84.90000000000001</v>
+        <v>0</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>1000</v>
@@ -4535,23 +4583,23 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>5648.47</v>
+        <v>0</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>2309.47</v>
+        <v>68.04000000000001</v>
       </c>
       <c r="E49" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>0</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="50">
@@ -4562,14 +4610,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>0</v>
+        <v>5648.47</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>0</v>
+        <v>2309.47</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0</v>
@@ -4578,7 +4626,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="51">
@@ -4589,7 +4637,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
@@ -4616,7 +4664,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
@@ -4643,7 +4691,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -4656,10 +4704,10 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -4670,11 +4718,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>-51.94</v>
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="n">
         <v>0</v>
@@ -4683,10 +4731,10 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>3000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="55">
@@ -4697,39 +4745,66 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>-51.94</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="2" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="n">
+      <c r="C56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
         <v>808.39</v>
       </c>
-      <c r="F55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" s="2" t="n">
+      <c r="F56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="56">
-      <c r="C56" s="6" t="n">
+    <row r="57">
+      <c r="C57" s="6" t="n">
         <v>48005.12</v>
       </c>
-      <c r="D56" s="6" t="n">
+      <c r="D57" s="6" t="n">
         <v>31281.76</v>
       </c>
-      <c r="E56" s="6" t="n">
+      <c r="E57" s="6" t="n">
         <v>50358.9</v>
       </c>
-      <c r="F56" s="6" t="n">
+      <c r="F57" s="6" t="n">
         <v>183.24</v>
       </c>
-      <c r="G56" s="6" t="n">
+      <c r="G57" s="6" t="n">
         <v>50500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-09 15:45:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LUI WONG ANGEL BOLIVAR</t>
+          <t>JUAREZ FLORES JORGE WILLIAMS</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MENA COSTA GUIDO LENNIN</t>
+          <t>LUI WONG ANGEL BOLIVAR</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MINUTOCORP S.A.</t>
+          <t>MENA COSTA GUIDO LENNIN</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
+          <t>MINUTOCORP S.A.</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MORALES GRACIELA ENITH</t>
+          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
+          <t>MORALES GRACIELA ENITH</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
+          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2419,7 +2419,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="L43" s="2" t="n">
-        <v>-59.72</v>
+        <v>0</v>
       </c>
       <c r="M43" s="2" t="n">
         <v>0</v>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="2" t="n">
-        <v>0</v>
+        <v>-59.72</v>
       </c>
       <c r="M44" s="2" t="n">
         <v>0</v>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -2803,7 +2803,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="L49" s="2" t="n">
-        <v>75.31999999999999</v>
+        <v>0</v>
       </c>
       <c r="M49" s="2" t="n">
         <v>0</v>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
@@ -2882,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="2" t="n">
-        <v>0</v>
+        <v>75.31999999999999</v>
       </c>
       <c r="M50" s="2" t="n">
         <v>0</v>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -3043,7 +3043,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -3074,7 +3074,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M54" s="2" t="n">
         <v>0</v>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M55" s="2" t="n">
         <v>0</v>
@@ -3139,105 +3139,153 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="C57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="D57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="E57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="F57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="G57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="H57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="I57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="J57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="K57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="L57" s="4" t="inlineStr">
-        <is>
-          <t>3 de 55</t>
-        </is>
-      </c>
-      <c r="M57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
-        </is>
-      </c>
-      <c r="N57" s="4" t="inlineStr">
-        <is>
-          <t>0 de 55</t>
+      <c r="C57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="D58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="H58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="I58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="J58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="K58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="L58" s="4" t="inlineStr">
+        <is>
+          <t>3 de 56</t>
+        </is>
+      </c>
+      <c r="M58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="N58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
         </is>
       </c>
     </row>
@@ -3252,7 +3300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4178,7 +4226,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>LUI WONG ANGEL BOLIVAR</t>
+          <t>JUAREZ FLORES JORGE WILLIAMS</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -4205,7 +4253,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MENA COSTA GUIDO LENNIN</t>
+          <t>LUI WONG ANGEL BOLIVAR</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -4232,7 +4280,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MINUTOCORP S.A.</t>
+          <t>MENA COSTA GUIDO LENNIN</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -4259,7 +4307,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
+          <t>MINUTOCORP S.A.</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -4275,7 +4323,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="2" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -4286,7 +4334,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MORALES GRACIELA ENITH</t>
+          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -4313,11 +4361,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
+          <t>MORALES GRACIELA ENITH</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>1875.17</v>
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>0</v>
@@ -4329,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="2" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="40">
@@ -4340,11 +4388,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
+          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>0</v>
+        <v>1875.17</v>
       </c>
       <c r="D40" s="2" t="n">
         <v>0</v>
@@ -4356,7 +4404,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="41">
@@ -4367,7 +4415,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -4394,7 +4442,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -4421,23 +4469,23 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>2078.33</v>
+        <v>0</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>3838.11</v>
+        <v>0</v>
       </c>
       <c r="E43" s="2" t="n">
-        <v>1167.85</v>
+        <v>0</v>
       </c>
       <c r="F43" s="2" t="n">
-        <v>-59.72</v>
+        <v>0</v>
       </c>
       <c r="G43" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -4448,23 +4496,23 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>1278.13</v>
+        <v>2078.33</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>1912.87</v>
+        <v>3838.11</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>737.72</v>
+        <v>1167.85</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>0</v>
+        <v>-59.72</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="45">
@@ -4475,23 +4523,23 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>0</v>
+        <v>1278.13</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>0</v>
+        <v>1912.87</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>0</v>
+        <v>737.72</v>
       </c>
       <c r="F45" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="46">
@@ -4502,7 +4550,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -4529,17 +4577,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>131.6</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>1709.57</v>
+        <v>0</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>598.58</v>
+        <v>0</v>
       </c>
       <c r="F47" s="2" t="n">
         <v>0</v>
@@ -4556,23 +4604,23 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>0</v>
+        <v>131.6</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>0</v>
+        <v>1709.57</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>3470.45</v>
+        <v>598.58</v>
       </c>
       <c r="F48" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G48" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -4583,20 +4631,20 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>68.04000000000001</v>
+        <v>0</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>0</v>
+        <v>3470.45</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>84.90000000000001</v>
+        <v>0</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>1000</v>
@@ -4610,23 +4658,23 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>5648.47</v>
+        <v>0</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>2309.47</v>
+        <v>68.04000000000001</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F50" s="2" t="n">
-        <v>0</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="51">
@@ -4637,14 +4685,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>0</v>
+        <v>5648.47</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>0</v>
+        <v>2309.47</v>
       </c>
       <c r="E51" s="2" t="n">
         <v>0</v>
@@ -4653,7 +4701,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="52">
@@ -4664,7 +4712,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
@@ -4691,7 +4739,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -4718,7 +4766,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -4731,10 +4779,10 @@
         <v>0</v>
       </c>
       <c r="F54" s="2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -4745,11 +4793,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
-        <v>-51.94</v>
+        <v>0</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>0</v>
@@ -4758,10 +4806,10 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>3000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="56">
@@ -4772,39 +4820,66 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>-51.94</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="2" t="n">
+      <c r="C57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="n">
         <v>808.39</v>
       </c>
-      <c r="F56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" s="2" t="n">
+      <c r="F57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="57">
-      <c r="C57" s="6" t="n">
+    <row r="58">
+      <c r="C58" s="6" t="n">
         <v>48005.12</v>
       </c>
-      <c r="D57" s="6" t="n">
+      <c r="D58" s="6" t="n">
         <v>31281.76</v>
       </c>
-      <c r="E57" s="6" t="n">
+      <c r="E58" s="6" t="n">
         <v>50358.9</v>
       </c>
-      <c r="F57" s="6" t="n">
+      <c r="F58" s="6" t="n">
         <v>183.24</v>
       </c>
-      <c r="G57" s="6" t="n">
+      <c r="G58" s="6" t="n">
         <v>50500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-11 09:10:11
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -941,10 +941,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>1699.51</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>332.71</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -965,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>226.6</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -3240,39 +3240,39 @@
       </c>
       <c r="E58" s="4" t="inlineStr">
         <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="F58" s="4" t="inlineStr">
+      <c r="H58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="G58" s="4" t="inlineStr">
+      <c r="I58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="H58" s="4" t="inlineStr">
+      <c r="J58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="I58" s="4" t="inlineStr">
+      <c r="K58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="J58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="K58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
       <c r="L58" s="4" t="inlineStr">
         <is>
           <t>3 de 56</t>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -3313,7 +3313,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -3591,7 +3591,7 @@
         <v>18249.33</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>2258.82</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>7000</v>
@@ -4877,7 +4877,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>183.24</v>
+        <v>2442.06</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -4905,8 +4905,8 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -5005,13 +5005,13 @@
         <v>142.502095025027</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>1699.51</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>142.502095025027</v>
+        <v>-1557.007904974973</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>11.92621062659832</v>
       </c>
     </row>
     <row r="5">
@@ -5053,13 +5053,13 @@
         <v>106.82</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>332.71</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>106.82</v>
+        <v>-225.89</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>3.114678899082569</v>
       </c>
     </row>
     <row r="7">
@@ -5317,13 +5317,13 @@
         <v>342</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>226.6</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>342</v>
+        <v>115.4</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>0.6625730994152047</v>
       </c>
     </row>
     <row r="18">
@@ -5360,13 +5360,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>183.24</v>
+        <v>2442.06</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>55226.46560036206</v>
+        <v>52967.64560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.003307001869340426</v>
+        <v>0.04407278424493277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-11 11:00:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1976,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="N31" s="2" t="n">
-        <v>0</v>
+        <v>1520.03</v>
       </c>
     </row>
     <row r="32">
@@ -2090,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0</v>
+        <v>814.08</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0</v>
@@ -3235,57 +3235,57 @@
       </c>
       <c r="D58" s="4" t="inlineStr">
         <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="E58" s="4" t="inlineStr">
+      <c r="H58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="I58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="J58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="K58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="L58" s="4" t="inlineStr">
+        <is>
+          <t>3 de 56</t>
+        </is>
+      </c>
+      <c r="M58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="F58" s="4" t="inlineStr">
+      <c r="N58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="G58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="H58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="I58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="J58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="K58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="L58" s="4" t="inlineStr">
-        <is>
-          <t>3 de 56</t>
-        </is>
-      </c>
-      <c r="M58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="N58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
         </is>
       </c>
     </row>
@@ -4158,7 +4158,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0</v>
+        <v>1520.03</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>0</v>
@@ -4239,7 +4239,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>0</v>
+        <v>814.08</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>0</v>
@@ -4877,7 +4877,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>2442.06</v>
+        <v>4776.17</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -4981,13 +4981,13 @@
         <v>4992.1832</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>814.08</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4992.1832</v>
+        <v>4178.1032</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.1630709385825424</v>
       </c>
     </row>
     <row r="4">
@@ -5341,13 +5341,13 @@
         <v>4130</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0</v>
+        <v>1520.03</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>4130</v>
+        <v>2609.97</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>0</v>
+        <v>0.368046004842615</v>
       </c>
     </row>
     <row r="19">
@@ -5360,13 +5360,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>2442.06</v>
+        <v>4776.17</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>52967.64560036206</v>
+        <v>50633.53560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.04407278424493277</v>
+        <v>0.08619735384352575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-13 17:30:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="2" t="n">
-        <v>0</v>
+        <v>1158.38</v>
       </c>
       <c r="M45" s="2" t="n">
         <v>0</v>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="L58" s="4" t="inlineStr">
         <is>
-          <t>3 de 56</t>
+          <t>4 de 56</t>
         </is>
       </c>
       <c r="M58" s="4" t="inlineStr">
@@ -4536,7 +4536,7 @@
         <v>737.72</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>0</v>
+        <v>1158.38</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>5000</v>
@@ -4877,7 +4877,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>4776.17</v>
+        <v>5934.55</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -4907,7 +4907,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5293,13 +5293,13 @@
         <v>38417.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>173.66</v>
+        <v>1332.04</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>38243.50999999999</v>
+        <v>37085.13</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.004520374613746926</v>
+        <v>0.0346730381233183</v>
       </c>
     </row>
     <row r="17">
@@ -5360,13 +5360,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>4776.17</v>
+        <v>5934.55</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50633.53560036206</v>
+        <v>49475.15560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.08619735384352575</v>
+        <v>0.107103077623304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-16 15:55:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2501,7 +2501,7 @@
         <v>814.08</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0</v>
+        <v>55.65</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0</v>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="E58" s="4" t="inlineStr">
         <is>
-          <t>1 de 56</t>
+          <t>2 de 56</t>
         </is>
       </c>
       <c r="F58" s="4" t="inlineStr">
@@ -4955,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>814.08</v>
+        <v>869.73</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>5934.55</v>
+        <v>5990.200000000001</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5721,13 +5721,13 @@
         <v>142.502095025027</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1699.51</v>
+        <v>1755.16</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-1557.007904974973</v>
+        <v>-1612.657904974973</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>11.92621062659832</v>
+        <v>12.31673120098164</v>
       </c>
     </row>
     <row r="5">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>5934.55</v>
+        <v>5990.2</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>49475.15560036207</v>
+        <v>49419.50560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.107103077623304</v>
+        <v>0.1081074143075912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-18 15:50:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3182,7 +3182,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="2" t="n">
-        <v>0</v>
+        <v>292.33</v>
       </c>
       <c r="M45" s="2" t="n">
         <v>1404.64</v>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="L58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="M58" s="4" t="inlineStr">
@@ -5252,7 +5252,7 @@
         <v>737.72</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>1404.64</v>
+        <v>1696.97</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>5000</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>6260.22</v>
+        <v>6552.55</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5985,13 +5985,13 @@
         <v>1505.12</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>292.33</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1505.12</v>
+        <v>1212.79</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>0.1942237163814181</v>
       </c>
     </row>
     <row r="16">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>6260.22</v>
+        <v>6552.55</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>49149.48560036207</v>
+        <v>48857.15560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1129805677935075</v>
+        <v>0.1182563583221273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-18 17:30:12
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>0</v>
+        <v>1140.48</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>0</v>
@@ -2057,10 +2057,10 @@
         <v>0</v>
       </c>
       <c r="Q26" s="2" t="n">
-        <v>0</v>
+        <v>7446.24</v>
       </c>
       <c r="R26" s="2" t="n">
-        <v>0</v>
+        <v>1531.2</v>
       </c>
     </row>
     <row r="27">
@@ -3931,77 +3931,77 @@
       </c>
       <c r="D58" s="4" t="inlineStr">
         <is>
+          <t>2 de 56</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>2 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="E58" s="4" t="inlineStr">
-        <is>
-          <t>2 de 56</t>
-        </is>
-      </c>
-      <c r="F58" s="4" t="inlineStr">
+      <c r="H58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="G58" s="4" t="inlineStr">
+      <c r="I58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="J58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="K58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="L58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="H58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="I58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="J58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="K58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="L58" s="4" t="inlineStr">
+      <c r="M58" s="4" t="inlineStr">
+        <is>
+          <t>5 de 56</t>
+        </is>
+      </c>
+      <c r="N58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="M58" s="4" t="inlineStr">
-        <is>
-          <t>5 de 56</t>
-        </is>
-      </c>
-      <c r="N58" s="4" t="inlineStr">
+      <c r="O58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="O58" s="4" t="inlineStr">
+      <c r="P58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="P58" s="4" t="inlineStr">
+      <c r="Q58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="Q58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
       <c r="R58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -4739,7 +4739,7 @@
         <v>8756.98</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>0</v>
+        <v>10117.92</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>5000</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>6552.55</v>
+        <v>16670.47</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5697,13 +5697,13 @@
         <v>4992.1832</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>814.08</v>
+        <v>1954.56</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4178.1032</v>
+        <v>3037.6232</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.1630709385825424</v>
+        <v>0.3915240931061985</v>
       </c>
     </row>
     <row r="4">
@@ -5937,13 +5937,13 @@
         <v>230</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0</v>
+        <v>1531.2</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>230</v>
+        <v>-1301.2</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>0</v>
+        <v>6.657391304347827</v>
       </c>
     </row>
     <row r="14">
@@ -5961,13 +5961,13 @@
         <v>483</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>7446.24</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>483</v>
+        <v>-6963.24</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0</v>
+        <v>15.41664596273292</v>
       </c>
     </row>
     <row r="15">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>6552.55</v>
+        <v>16670.47</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>48857.15560036207</v>
+        <v>38739.23560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1182563583221273</v>
+        <v>0.300858303060377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-20 17:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0</v>
+        <v>1534.46</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>0</v>
@@ -3926,7 +3926,7 @@
     <row r="58">
       <c r="C58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="D58" s="4" t="inlineStr">
@@ -4307,7 +4307,7 @@
         <v>18249.33</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>2258.82</v>
+        <v>3793.28</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>7000</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>21515.25</v>
+        <v>23049.71</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5673,13 +5673,13 @@
         <v>672.340305337043</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>1534.46</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>672.340305337043</v>
+        <v>-862.119694662957</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0</v>
+        <v>2.282266863698998</v>
       </c>
     </row>
     <row r="3">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>21515.25</v>
+        <v>23049.71</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>33894.45560036207</v>
+        <v>32359.99560036208</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.3882938876300294</v>
+        <v>0.4159868699942955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-24 12:50:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -617,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>1115.1</v>
+        <v>669.0599999999999</v>
       </c>
       <c r="R2" s="2" t="n">
         <v>261</v>
@@ -4091,7 +4091,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1376.1</v>
+        <v>930.0599999999999</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>1500</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>23049.71</v>
+        <v>22603.67</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5961,13 +5961,13 @@
         <v>483</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>8561.34</v>
+        <v>8115.3</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>-8078.34</v>
+        <v>-7632.3</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>17.72534161490683</v>
+        <v>16.80186335403727</v>
       </c>
     </row>
     <row r="15">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>23049.71</v>
+        <v>22603.67</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>32359.99560036208</v>
+        <v>32806.03560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4159868699942955</v>
+        <v>0.4079370167209894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 17:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0</v>
+        <v>559.83</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
@@ -3936,7 +3936,7 @@
       </c>
       <c r="E58" s="4" t="inlineStr">
         <is>
-          <t>2 de 56</t>
+          <t>3 de 56</t>
         </is>
       </c>
       <c r="F58" s="4" t="inlineStr">
@@ -4118,7 +4118,7 @@
         <v>3316.15</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>559.83</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>1500</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>22603.67</v>
+        <v>23163.5</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5721,13 +5721,13 @@
         <v>142.502095025027</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1755.16</v>
+        <v>2314.99</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-1612.657904974973</v>
+        <v>-2172.487904974973</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>12.31673120098164</v>
+        <v>16.24530502231163</v>
       </c>
     </row>
     <row r="5">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>22603.67</v>
+        <v>23163.5</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>32806.03560036207</v>
+        <v>32246.20560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4079370167209894</v>
+        <v>0.4180404813385011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-26 15:25:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2873,7 +2873,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>0</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="J40" s="2" t="n">
         <v>0</v>
@@ -3956,7 +3956,7 @@
       </c>
       <c r="I58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="J58" s="4" t="inlineStr">
@@ -5117,7 +5117,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>0</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>1000</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>25320.04</v>
+        <v>25406.44</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5817,13 +5817,13 @@
         <v>750</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>750</v>
+        <v>663.6</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0</v>
+        <v>0.1152</v>
       </c>
     </row>
     <row r="9">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>25320.03999999999</v>
+        <v>25406.44</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>30089.66560036207</v>
+        <v>30003.26560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4569603777110583</v>
+        <v>0.458519671323321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-30 13:45:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>0</v>
+        <v>36.55</v>
       </c>
       <c r="J26" s="2" t="n">
         <v>0</v>
@@ -3098,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>0</v>
+        <v>1112.84</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>0</v>
@@ -3533,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="2" t="n">
-        <v>0</v>
+        <v>779.4</v>
       </c>
       <c r="J51" s="2" t="n">
         <v>0</v>
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="O51" s="2" t="n">
-        <v>0</v>
+        <v>3040.06</v>
       </c>
       <c r="P51" s="2" t="n">
         <v>0</v>
@@ -3931,62 +3931,62 @@
       </c>
       <c r="D58" s="4" t="inlineStr">
         <is>
+          <t>3 de 56</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>3 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="H58" s="4" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="I58" s="4" t="inlineStr">
+        <is>
+          <t>4 de 56</t>
+        </is>
+      </c>
+      <c r="J58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="K58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="L58" s="4" t="inlineStr">
+        <is>
           <t>2 de 56</t>
         </is>
       </c>
-      <c r="E58" s="4" t="inlineStr">
-        <is>
-          <t>3 de 56</t>
-        </is>
-      </c>
-      <c r="F58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="G58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="H58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="I58" s="4" t="inlineStr">
+      <c r="M58" s="4" t="inlineStr">
+        <is>
+          <t>7 de 56</t>
+        </is>
+      </c>
+      <c r="N58" s="4" t="inlineStr">
         <is>
           <t>2 de 56</t>
         </is>
       </c>
-      <c r="J58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="K58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="L58" s="4" t="inlineStr">
+      <c r="O58" s="4" t="inlineStr">
         <is>
           <t>2 de 56</t>
-        </is>
-      </c>
-      <c r="M58" s="4" t="inlineStr">
-        <is>
-          <t>7 de 56</t>
-        </is>
-      </c>
-      <c r="N58" s="4" t="inlineStr">
-        <is>
-          <t>2 de 56</t>
-        </is>
-      </c>
-      <c r="O58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
         </is>
       </c>
       <c r="P58" s="4" t="inlineStr">
@@ -4739,7 +4739,7 @@
         <v>8756.98</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>15743.14</v>
+        <v>15779.69</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>5000</v>
@@ -5225,7 +5225,7 @@
         <v>1167.85</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>-59.72</v>
+        <v>1053.12</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>2000</v>
@@ -5414,7 +5414,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>0</v>
+        <v>3819.46</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>3000</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>29573.5</v>
+        <v>34542.35</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5697,13 +5697,13 @@
         <v>4992.1832</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1954.56</v>
+        <v>3067.4</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>3037.6232</v>
+        <v>1924.7832</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.3915240931061985</v>
+        <v>0.6144405918436647</v>
       </c>
     </row>
     <row r="4">
@@ -5721,13 +5721,13 @@
         <v>142.502095025027</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2314.99</v>
+        <v>2379.81</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-2172.487904974973</v>
+        <v>-2237.307904974973</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>16.24530502231163</v>
+        <v>16.70017552781975</v>
       </c>
     </row>
     <row r="5">
@@ -5817,13 +5817,13 @@
         <v>750</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>825.9</v>
+        <v>1641.85</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-75.89999999999998</v>
+        <v>-891.8499999999999</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>1.1012</v>
+        <v>2.189133333333333</v>
       </c>
     </row>
     <row r="9">
@@ -5937,13 +5937,13 @@
         <v>230</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>1792.2</v>
+        <v>1802.64</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>-1562.2</v>
+        <v>-1572.64</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>7.792173913043478</v>
+        <v>7.837565217391305</v>
       </c>
     </row>
     <row r="14">
@@ -6057,13 +6057,13 @@
         <v>4130</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>1520.03</v>
+        <v>4560.09</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>2609.97</v>
+        <v>-430.0900000000001</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>0.368046004842615</v>
+        <v>1.104138014527845</v>
       </c>
     </row>
     <row r="19">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>29573.5</v>
+        <v>34617.61</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>25836.20560036207</v>
+        <v>20792.09560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5337241856741927</v>
+        <v>0.6247571544537099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-30 13:50:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -620,7 +620,7 @@
         <v>669.0599999999999</v>
       </c>
       <c r="R2" s="2" t="n">
-        <v>261</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3">
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>612.86</v>
+        <v>5465.6</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>2042.06</v>
@@ -4091,7 +4091,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>930.0599999999999</v>
+        <v>1191.06</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>1500</v>
@@ -4469,7 +4469,7 @@
         <v>6711.78</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>4167.06</v>
+        <v>9019.799999999999</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>3000</v>
@@ -5593,7 +5593,7 @@
         <v>50358.9</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>34542.35</v>
+        <v>39656.09</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>
@@ -5937,13 +5937,13 @@
         <v>230</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>1802.64</v>
+        <v>2063.64</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>-1572.64</v>
+        <v>-1833.64</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>7.837565217391305</v>
+        <v>8.972347826086956</v>
       </c>
     </row>
     <row r="14">
@@ -6009,13 +6009,13 @@
         <v>38417.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>4371.46</v>
+        <v>9224.200000000001</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>34045.71</v>
+        <v>29192.97</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1137892249741457</v>
+        <v>0.2401061816890729</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>34617.61</v>
+        <v>39731.35000000001</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>20792.09560036207</v>
+        <v>15678.35560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.6247571544537099</v>
+        <v>0.7170467622867209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-01 15:05:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>0</v>
+        <v>793.77</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -4029,7 +4029,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="11" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -4766,7 +4766,7 @@
         <v>714.15</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0</v>
+        <v>793.77</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>0</v>
+        <v>793.77</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>50500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-07-03 13:15:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>0</v>
+        <v>-134.78</v>
       </c>
       <c r="N26" s="2" t="n">
         <v>0</v>
@@ -4029,7 +4029,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -4739,7 +4739,7 @@
         <v>15779.69</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>0</v>
+        <v>-134.78</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>3000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>793.77</v>
+        <v>658.99</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>793.77</v>
+        <v>658.99</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>39596.4</v>
+        <v>39731.18</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.01965255407441959</v>
+        <v>0.01631560352432287</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>793.77</v>
+        <v>658.99</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>54615.93560036207</v>
+        <v>54750.71560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.01432546864127019</v>
+        <v>0.0118930427956595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-04 17:05:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>1451.52</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>1 de 56</t>
+          <t>2 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -4307,7 +4307,7 @@
         <v>3793.28</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>1451.52</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>10000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>658.99</v>
+        <v>2110.51</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5621,8 +5621,8 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -5721,13 +5721,13 @@
         <v>142.502095025027</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>275.59</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>142.502095025027</v>
+        <v>-133.087904974973</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>1.933936479681926</v>
       </c>
     </row>
     <row r="5">
@@ -5817,13 +5817,13 @@
         <v>750</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>779.4</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>750</v>
+        <v>-29.39999999999998</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0</v>
+        <v>1.0392</v>
       </c>
     </row>
     <row r="9">
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>658.99</v>
+        <v>2110.51</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>39731.18</v>
+        <v>38279.66</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.01631560352432287</v>
+        <v>0.05225306058380047</v>
       </c>
     </row>
     <row r="17">
@@ -6033,13 +6033,13 @@
         <v>342</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>372.66</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>342</v>
+        <v>-30.66000000000003</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>1.089649122807018</v>
       </c>
     </row>
     <row r="18">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>658.99</v>
+        <v>3538.16</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>54750.71560036207</v>
+        <v>51871.54560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.0118930427956595</v>
+        <v>0.06385451721253831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-07 16:50:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>2 de 56</t>
+          <t>3 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -4118,7 +4118,7 @@
         <v>559.83</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>3500</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>3538.16</v>
+        <v>3637.81</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2110.51</v>
+        <v>2210.16</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>38279.66</v>
+        <v>38180.00999999999</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.05225306058380047</v>
+        <v>0.05472024504972373</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3538.16</v>
+        <v>3637.809999999999</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51871.54560036207</v>
+        <v>51771.89560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.06385451721253831</v>
+        <v>0.06565293860677412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-08 09:15:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2222,7 +2222,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="2" t="n">
-        <v>0</v>
+        <v>1392.03</v>
       </c>
       <c r="M29" s="2" t="n">
         <v>0</v>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="L58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="M58" s="4" t="inlineStr">
@@ -4820,7 +4820,7 @@
         <v>23.76</v>
       </c>
       <c r="F29" s="2" t="n">
-        <v>0</v>
+        <v>1392.03</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>2000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>3637.81</v>
+        <v>5029.84</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5985,13 +5985,13 @@
         <v>1505.12</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>1392.03</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1505.12</v>
+        <v>113.0899999999999</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>0.9248631338365048</v>
       </c>
     </row>
     <row r="16">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3637.809999999999</v>
+        <v>5029.84</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51771.89560036206</v>
+        <v>50379.86560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.06565293860677412</v>
+        <v>0.09077543267017707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-08 15:10:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>1451.52</v>
+        <v>1428.84</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -4307,7 +4307,7 @@
         <v>3793.28</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>1451.52</v>
+        <v>1428.84</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>10000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>5029.84</v>
+        <v>5007.16</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5623,7 +5623,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2210.16</v>
+        <v>2187.48</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>38180.00999999999</v>
+        <v>38202.69</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.05472024504972373</v>
+        <v>0.0541587222831694</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>5029.84</v>
+        <v>5007.16</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50379.86560036206</v>
+        <v>50402.54560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.09077543267017707</v>
+        <v>0.09036611809695812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-08 16:35:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3185,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>0</v>
+        <v>423.78</v>
       </c>
       <c r="N45" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>3 de 56</t>
+          <t>4 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -5252,7 +5252,7 @@
         <v>1696.97</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>0</v>
+        <v>423.78</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>4000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>5007.16</v>
+        <v>5430.94</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5623,7 +5623,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2187.48</v>
+        <v>2611.26</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>38202.69</v>
+        <v>37778.91</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.0541587222831694</v>
+        <v>0.06465087916193471</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>5007.16</v>
+        <v>5430.940000000001</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50402.54560036207</v>
+        <v>49978.76560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.09036611809695812</v>
+        <v>0.0980142366965493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-09 09:25:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="2" t="n">
-        <v>0</v>
+        <v>184.73</v>
       </c>
       <c r="N31" s="2" t="n">
         <v>0</v>
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="P31" s="2" t="n">
-        <v>0</v>
+        <v>23.16</v>
       </c>
       <c r="Q31" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>4 de 56</t>
+          <t>5 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="P58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="Q58" s="4" t="inlineStr">
@@ -4874,7 +4874,7 @@
         <v>4575.95</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0</v>
+        <v>207.89</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>5430.94</v>
+        <v>5638.83</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5865,13 +5865,13 @@
         <v>650.25</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>23.16</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>650.25</v>
+        <v>627.09</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0</v>
+        <v>0.03561707035755479</v>
       </c>
     </row>
     <row r="11">
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2611.26</v>
+        <v>2795.99</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>37778.91</v>
+        <v>37594.18</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.06465087916193471</v>
+        <v>0.06922451675741895</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>5430.940000000001</v>
+        <v>5638.83</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>49978.76560036207</v>
+        <v>49770.87560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.0980142366965493</v>
+        <v>0.1017661064772586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-09 15:20:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="P31" s="2" t="n">
-        <v>23.16</v>
+        <v>22.56</v>
       </c>
       <c r="Q31" s="2" t="n">
         <v>0</v>
@@ -4874,7 +4874,7 @@
         <v>4575.95</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>207.89</v>
+        <v>207.29</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>5638.83</v>
+        <v>5638.23</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5865,13 +5865,13 @@
         <v>650.25</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>23.16</v>
+        <v>22.56</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>627.09</v>
+        <v>627.6900000000001</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0.03561707035755479</v>
+        <v>0.03469434832756632</v>
       </c>
     </row>
     <row r="11">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>5638.83</v>
+        <v>5638.23</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>49770.87560036207</v>
+        <v>49771.47560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1017661064772586</v>
+        <v>0.1017552780493957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-10 08:50:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2795.99</v>
+        <v>4911.69</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>37594.18</v>
+        <v>35478.48</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.06922451675741895</v>
+        <v>0.1216060739531426</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>5638.23</v>
+        <v>7753.929999999999</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>49771.47560036207</v>
+        <v>47655.77560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1017552780493957</v>
+        <v>0.1399381194320825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-10 08:55:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>-134.78</v>
+        <v>1980.92</v>
       </c>
       <c r="N26" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>5 de 56</t>
+          <t>6 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -4739,7 +4739,7 @@
         <v>15779.69</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>-134.78</v>
+        <v>1980.92</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>3000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>5638.23</v>
+        <v>7753.93</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-07-15 15:00:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>99.65000000000001</v>
+        <v>3337.3</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -4118,7 +4118,7 @@
         <v>559.83</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>99.65000000000001</v>
+        <v>3337.3</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>3500</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>7753.93</v>
+        <v>10991.58</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>4911.69</v>
+        <v>8149.34</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>35478.48</v>
+        <v>32240.83</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1216060739531426</v>
+        <v>0.2017654295587268</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>7753.929999999999</v>
+        <v>10991.58</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>47655.77560036207</v>
+        <v>44418.12560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1399381194320825</v>
+        <v>0.1983692185494697</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-15 15:05:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2498,10 +2498,10 @@
         <v>0</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0</v>
+        <v>915.84</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0</v>
+        <v>124.78</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0</v>
@@ -2510,10 +2510,10 @@
         <v>0</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>0</v>
+        <v>137.46</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>0</v>
+        <v>49.28</v>
       </c>
       <c r="J34" s="2" t="n">
         <v>0</v>
@@ -3931,32 +3931,32 @@
       </c>
       <c r="D58" s="4" t="inlineStr">
         <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="inlineStr">
+        <is>
+          <t>2 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="E58" s="4" t="inlineStr">
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>0 de 56</t>
+        </is>
+      </c>
+      <c r="H58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
         </is>
       </c>
-      <c r="F58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="G58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="H58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
       <c r="I58" s="4" t="inlineStr">
         <is>
-          <t>1 de 56</t>
+          <t>2 de 56</t>
         </is>
       </c>
       <c r="J58" s="4" t="inlineStr">
@@ -4955,7 +4955,7 @@
         <v>869.73</v>
       </c>
       <c r="F34" s="2" t="n">
-        <v>0</v>
+        <v>1227.36</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>10991.58</v>
+        <v>12218.94</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5697,13 +5697,13 @@
         <v>4992.1832</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>915.84</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4992.1832</v>
+        <v>4076.3432</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.1834548059053602</v>
       </c>
     </row>
     <row r="4">
@@ -5721,13 +5721,13 @@
         <v>142.502095025027</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>275.59</v>
+        <v>400.37</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-133.087904974973</v>
+        <v>-257.867904974973</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>1.933936479681926</v>
+        <v>2.809572728946089</v>
       </c>
     </row>
     <row r="5">
@@ -5793,13 +5793,13 @@
         <v>2300</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>137.46</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2300</v>
+        <v>2162.54</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>0.05976521739130435</v>
       </c>
     </row>
     <row r="8">
@@ -5817,13 +5817,13 @@
         <v>750</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>779.4</v>
+        <v>828.6799999999999</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-29.39999999999998</v>
+        <v>-78.67999999999995</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>1.0392</v>
+        <v>1.104906666666667</v>
       </c>
     </row>
     <row r="9">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>10991.58</v>
+        <v>12218.94</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44418.12560036207</v>
+        <v>43190.76560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1983692185494697</v>
+        <v>0.22051985058589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-16 15:40:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3425,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="2" t="n">
-        <v>0</v>
+        <v>616.41</v>
       </c>
       <c r="N49" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>6 de 56</t>
+          <t>7 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -5360,7 +5360,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="n">
-        <v>0</v>
+        <v>616.41</v>
       </c>
       <c r="G49" s="2" t="n">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>12218.94</v>
+        <v>12835.35</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>8149.34</v>
+        <v>8765.75</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>32240.83</v>
+        <v>31624.42</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2017654295587268</v>
+        <v>0.2170268161782929</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>12218.94</v>
+        <v>12835.35</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>43190.76560036207</v>
+        <v>42574.35560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.22051985058589</v>
+        <v>0.2316444359508766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-17 08:30:07
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3185,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>423.78</v>
+        <v>676.34</v>
       </c>
       <c r="N45" s="2" t="n">
         <v>0</v>
@@ -5252,7 +5252,7 @@
         <v>1696.97</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>423.78</v>
+        <v>676.34</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>4000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>12835.35</v>
+        <v>13087.91</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>8765.75</v>
+        <v>9018.309999999999</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>31624.42</v>
+        <v>31371.86</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2170268161782929</v>
+        <v>0.2232798227885646</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>12835.35</v>
+        <v>13087.91</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>42574.35560036206</v>
+        <v>42321.79560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2316444359508766</v>
+        <v>0.2362024821859815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-17 15:00:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>3337.3</v>
+        <v>6510.91</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -4118,7 +4118,7 @@
         <v>559.83</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>3337.3</v>
+        <v>6510.91</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>3500</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>13087.91</v>
+        <v>16261.52</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5621,7 +5621,7 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>9018.309999999999</v>
+        <v>12191.92</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>31371.86</v>
+        <v>28198.25</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2232798227885646</v>
+        <v>0.3018536440921145</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>13087.91</v>
+        <v>16261.52</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>42321.79560036206</v>
+        <v>39148.18560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2362024821859815</v>
+        <v>0.2934778271027981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-18 14:05:10
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="O51" s="2" t="n">
-        <v>0</v>
+        <v>-11.52</v>
       </c>
       <c r="P51" s="2" t="n">
         <v>0</v>
@@ -5414,7 +5414,7 @@
         <v>3819.46</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>0</v>
+        <v>-11.52</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>2000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>17050.95</v>
+        <v>17039.43</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5623,7 +5623,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6057,13 +6057,13 @@
         <v>2300</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0</v>
+        <v>-11.52</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>2300</v>
+        <v>2311.52</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>0</v>
+        <v>-0.005008695652173913</v>
       </c>
     </row>
     <row r="19">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>17050.95</v>
+        <v>17039.43</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>38358.75560036207</v>
+        <v>38370.27560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.3077249701158597</v>
+        <v>0.3075170643008913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-18 17:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0</v>
+        <v>1186.06</v>
       </c>
       <c r="N6" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>7 de 56</t>
+          <t>8 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -4199,7 +4199,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>1186.06</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>2000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>17039.43</v>
+        <v>18225.49</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>12191.92</v>
+        <v>13377.98</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>28198.25</v>
+        <v>27012.19</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.3018536440921145</v>
+        <v>0.331218709898968</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>17039.43</v>
+        <v>18225.49</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>38370.27560036207</v>
+        <v>37184.21560036206</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.3075170643008913</v>
+        <v>0.3289223395527462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-28 15:50:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2102,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>0</v>
+        <v>440.99</v>
       </c>
       <c r="M27" s="2" t="n">
         <v>793.77</v>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="L58" s="4" t="inlineStr">
         <is>
-          <t>1 de 56</t>
+          <t>2 de 56</t>
         </is>
       </c>
       <c r="M58" s="4" t="inlineStr">
@@ -4766,7 +4766,7 @@
         <v>714.15</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>793.77</v>
+        <v>1234.76</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>2000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>23931.39</v>
+        <v>24372.38</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -5985,13 +5985,13 @@
         <v>1505.12</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>1392.03</v>
+        <v>1833.02</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>113.0899999999999</v>
+        <v>-327.9000000000001</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.9248631338365048</v>
+        <v>1.217856383544169</v>
       </c>
     </row>
     <row r="16">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>23992.97</v>
+        <v>24433.96</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>31416.73560036207</v>
+        <v>30975.74560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4330102414376159</v>
+        <v>0.4409689554430756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-31 12:45:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>1428.84</v>
+        <v>2614.89</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -4307,7 +4307,7 @@
         <v>3793.28</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>1428.84</v>
+        <v>2614.89</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>10000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>36289.64</v>
+        <v>37475.69</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>26362.77</v>
+        <v>27548.82</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>14027.4</v>
+        <v>12841.35</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.6527026254160356</v>
+        <v>0.6820674436378951</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>36351.22000000001</v>
+        <v>37537.27000000001</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>19058.48560036207</v>
+        <v>17872.43560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.6560442724994821</v>
+        <v>0.6774493672775393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-31 12:50:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>2614.89</v>
+        <v>24572.5</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -3125,7 +3125,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="2" t="n">
-        <v>0</v>
+        <v>1186.08</v>
       </c>
       <c r="N44" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>11 de 56</t>
+          <t>12 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -4307,7 +4307,7 @@
         <v>3793.28</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>2614.89</v>
+        <v>24572.5</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>10000</v>
@@ -5225,7 +5225,7 @@
         <v>1053.12</v>
       </c>
       <c r="F44" s="2" t="n">
-        <v>0</v>
+        <v>1186.08</v>
       </c>
       <c r="G44" s="2" t="n">
         <v>1000</v>
@@ -5593,7 +5593,7 @@
         <v>43293.1</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>37475.69</v>
+        <v>60619.38</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>54500</v>
@@ -6009,13 +6009,13 @@
         <v>40390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>27548.82</v>
+        <v>50692.51</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>12841.35</v>
+        <v>-10302.34</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.6820674436378951</v>
+        <v>1.255070478782337</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>55409.70560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>37537.27000000001</v>
+        <v>60680.96000000001</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>17872.43560036207</v>
+        <v>-5271.25439963793</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.6774493672775393</v>
+        <v>1.095132330022766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 14:10:10
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3185,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>0</v>
+        <v>94.56</v>
       </c>
       <c r="N45" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -5252,7 +5252,7 @@
         <v>785.08</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>0</v>
+        <v>94.56</v>
       </c>
       <c r="G45" s="2" t="n">
         <v>4500</v>
@@ -5593,7 +5593,7 @@
         <v>64672.74</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>68495.12999999999</v>
+        <v>68589.68999999999</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>57000</v>
@@ -5621,9 +5621,9 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="27" customWidth="1" min="6" max="6"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6009,13 +6009,13 @@
         <v>50390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>16.27</v>
+        <v>110.83</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>50373.9</v>
+        <v>50279.34</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.0003228804348149649</v>
+        <v>0.002199436913985406</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>16.27</v>
+        <v>110.83</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>65338.83560036207</v>
+        <v>65244.27560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.0002489476506929531</v>
+        <v>0.001695812423251382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 14:15:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2102,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>0</v>
+        <v>114.77</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>0</v>
@@ -3971,12 +3971,12 @@
       </c>
       <c r="L58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>1 de 56</t>
+          <t>2 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -4766,7 +4766,7 @@
         <v>1212.58</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>0</v>
+        <v>261.77</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>2000</v>
@@ -5593,7 +5593,7 @@
         <v>64672.74</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>68589.68999999999</v>
+        <v>68851.45999999999</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>57000</v>
@@ -5621,7 +5621,7 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
@@ -5985,13 +5985,13 @@
         <v>1505.12</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1505.12</v>
+        <v>1358.12</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>0.09766663123206124</v>
       </c>
     </row>
     <row r="16">
@@ -6009,13 +6009,13 @@
         <v>50390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>110.83</v>
+        <v>225.6</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>50279.34</v>
+        <v>50164.57</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.002199436913985406</v>
+        <v>0.004477063681269581</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>110.83</v>
+        <v>372.6</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>65244.27560036207</v>
+        <v>64982.50560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.001695812423251382</v>
+        <v>0.005701161318266401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 15:30:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>-60.08</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -4307,7 +4307,7 @@
         <v>24572.5</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>-60.08</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>8000</v>
@@ -5593,7 +5593,7 @@
         <v>64672.74</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>68851.45999999999</v>
+        <v>68791.37999999999</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>57000</v>
@@ -5621,7 +5621,7 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
@@ -6009,13 +6009,13 @@
         <v>50390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>225.6</v>
+        <v>165.52</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>50164.57</v>
+        <v>50224.65</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.004477063681269581</v>
+        <v>0.003284767644165519</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>372.6</v>
+        <v>312.52</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>64982.50560036207</v>
+        <v>65042.58560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.005701161318266401</v>
+        <v>0.00478187583248689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-06 15:45:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>-60.08</v>
+        <v>-78.61</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -4307,7 +4307,7 @@
         <v>24572.5</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-60.08</v>
+        <v>-78.61</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>8000</v>
@@ -5593,7 +5593,7 @@
         <v>64672.74</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>68791.37999999999</v>
+        <v>68772.84999999999</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>57000</v>
@@ -6009,13 +6009,13 @@
         <v>50390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>165.52</v>
+        <v>146.99</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>50224.65</v>
+        <v>50243.18</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.003284767644165519</v>
+        <v>0.002917037191976134</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>312.52</v>
+        <v>293.99</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>65042.58560036207</v>
+        <v>65061.11560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.00478187583248689</v>
+        <v>0.004498347868913417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-08 16:35:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1061,13 +1061,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>2237.88</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0</v>
+        <v>122.1</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>0</v>
@@ -1088,7 +1088,7 @@
         <v>-78.61</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0</v>
+        <v>453.2</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>0</v>
@@ -3936,39 +3936,39 @@
       </c>
       <c r="E58" s="4" t="inlineStr">
         <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="F58" s="4" t="inlineStr">
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>1 de 56</t>
+        </is>
+      </c>
+      <c r="H58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="G58" s="4" t="inlineStr">
+      <c r="I58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="H58" s="4" t="inlineStr">
+      <c r="J58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="I58" s="4" t="inlineStr">
+      <c r="K58" s="4" t="inlineStr">
         <is>
           <t>0 de 56</t>
         </is>
       </c>
-      <c r="J58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="K58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
       <c r="L58" s="4" t="inlineStr">
         <is>
           <t>1 de 56</t>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="N58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="O58" s="4" t="inlineStr">
@@ -4307,7 +4307,7 @@
         <v>24572.5</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-78.61</v>
+        <v>2734.57</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>8000</v>
@@ -5593,7 +5593,7 @@
         <v>64672.74</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>68821.75999999999</v>
+        <v>71634.93999999999</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>57000</v>
@@ -5621,8 +5621,8 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -5721,13 +5721,13 @@
         <v>142.502095025027</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>2237.88</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>142.502095025027</v>
+        <v>-2095.377904974973</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>15.70419017072676</v>
       </c>
     </row>
     <row r="5">
@@ -5769,13 +5769,13 @@
         <v>106.82</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>122.1</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>106.82</v>
+        <v>-15.28</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>1.143044373712788</v>
       </c>
     </row>
     <row r="7">
@@ -6033,13 +6033,13 @@
         <v>342</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>453.2</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>342</v>
+        <v>-111.2</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>1.325146198830409</v>
       </c>
     </row>
     <row r="18">
@@ -6076,13 +6076,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>342.9</v>
+        <v>3156.08</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>65012.20560036207</v>
+        <v>62199.02560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.005246720923332122</v>
+        <v>0.04829125392741337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-14 11:30:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="2" t="n">
-        <v>0</v>
+        <v>4275.73</v>
       </c>
       <c r="N56" s="2" t="n">
         <v>0</v>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="M58" s="4" t="inlineStr">
         <is>
-          <t>3 de 56</t>
+          <t>4 de 56</t>
         </is>
       </c>
       <c r="N58" s="4" t="inlineStr">
@@ -5549,7 +5549,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>0</v>
+        <v>4275.73</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>5000</v>
@@ -5593,7 +5593,7 @@
         <v>64672.74</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>74512.17999999999</v>
+        <v>78787.90999999999</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>57000</v>
@@ -5623,7 +5623,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6009,13 +6009,13 @@
         <v>50390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>195.9</v>
+        <v>4471.63</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>50194.27</v>
+        <v>45918.54</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.003887663010464144</v>
+        <v>0.08874012530618572</v>
       </c>
     </row>
     <row r="17">
@@ -6076,13 +6076,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>6033.32</v>
+        <v>10309.05</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>59321.78560036207</v>
+        <v>55046.05560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.09231597049039998</v>
+        <v>0.1577390152658997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-19 17:10:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0</v>
+        <v>179.1</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="D58" s="4" t="inlineStr">
         <is>
-          <t>0 de 56</t>
+          <t>1 de 56</t>
         </is>
       </c>
       <c r="E58" s="4" t="inlineStr">
@@ -4604,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0</v>
+        <v>179.1</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>0</v>
@@ -5593,7 +5593,7 @@
         <v>64672.74</v>
       </c>
       <c r="F58" s="6" t="n">
-        <v>78787.90999999999</v>
+        <v>78967.00999999999</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>57000</v>
@@ -5697,13 +5697,13 @@
         <v>5437.5832</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>179.1</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>5437.5832</v>
+        <v>5258.4832</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.03293742705398972</v>
       </c>
     </row>
     <row r="4">
@@ -6076,13 +6076,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>10309.05</v>
+        <v>10488.15</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>55046.05560036207</v>
+        <v>54866.95560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1577390152658997</v>
+        <v>0.160479428556564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-20 12:25:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ALVAREZ SAAVEDRA EDWIN GEOVANNY</t>
+          <t>ALTAMIRANO VILLAVICENCIO JUAN ALEJANDRO</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -751,7 +751,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ANGAMARCA CURIPONA WILMA</t>
+          <t>ALVAREZ SAAVEDRA EDWIN GEOVANNY</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -811,7 +811,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ARIAS MEZA RONALD FABRICIO</t>
+          <t>ANGAMARCA CURIPONA WILMA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>2003.44</v>
+        <v>0</v>
       </c>
       <c r="P6" s="2" t="n">
         <v>0</v>
@@ -871,7 +871,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ARMIJOS SALINAS LUIS CLAUDIO</t>
+          <t>ARIAS MEZA RONALD FABRICIO</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>0</v>
+        <v>2003.44</v>
       </c>
       <c r="P7" s="2" t="n">
         <v>0</v>
@@ -931,7 +931,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ARREAGA DELGADO ITALO TEOBALDO</t>
+          <t>ARMIJOS SALINAS LUIS CLAUDIO</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -991,7 +991,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BADILLO VERGARA MARIELA MARIA</t>
+          <t>ARREAGA DELGADO ITALO TEOBALDO</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BORJA TORRES LETTY JANET</t>
+          <t>BADILLO VERGARA MARIELA MARIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1061,13 +1061,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>2237.88</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>122.1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
         <v>0</v>
@@ -1085,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>-78.61</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>453.2</v>
+        <v>0</v>
       </c>
       <c r="O10" s="2" t="n">
         <v>0</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BRIONES DIAZ HECTOR FERNANDO</t>
+          <t>BORJA TORRES LETTY JANET</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1121,13 +1121,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0</v>
+        <v>2237.88</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0</v>
+        <v>122.1</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>0</v>
@@ -1145,10 +1145,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>-78.61</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>0</v>
+        <v>453.2</v>
       </c>
       <c r="O11" s="2" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BUENAÑO VITERI MARJORIE LETICIA</t>
+          <t>BRIONES DIAZ HECTOR FERNANDO</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1202,10 +1202,10 @@
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>873.8</v>
+        <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>-23.02</v>
+        <v>0</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CALERO LOPEZ GISELLA JACKELINE</t>
+          <t>BUENAÑO VITERI MARJORIE LETICIA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1262,10 +1262,10 @@
         <v>0</v>
       </c>
       <c r="L13" s="2" t="n">
-        <v>0</v>
+        <v>873.8</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>-23.02</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CARREÑO SANCHEZ ITALO VICENTE</t>
+          <t>CALERO LOPEZ GISELLA JACKELINE</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CASA FERRETERIA FONG S.A. FERREFONG</t>
+          <t>CARREÑO SANCHEZ ITALO VICENTE</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CHASI PASTO ANGEL NOLBERTO</t>
+          <t>CASA FERRETERIA FONG S.A. FERREFONG</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>COMERCIALIZADORA &amp; CONSTRUCTORA ELECTRICA PALAU &amp; ORTIZ MEGA-ENERGYCORP SA</t>
+          <t>CHASI PASTO ANGEL NOLBERTO</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>COMERCIALIZADORA RAMIREZ GALVAN CIA. LTDA</t>
+          <t>COMERCIALIZADORA &amp; CONSTRUCTORA ELECTRICA PALAU &amp; ORTIZ MEGA-ENERGYCORP SA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CONTRATISTAS ACABADOS PARA LA CONTRUCCION JANDRI S.A.</t>
+          <t>COMERCIALIZADORA RAMIREZ GALVAN CIA. LTDA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>COZZARELLI CONTRERAS FATIMA MERCEDES</t>
+          <t>CONTRATISTAS ACABADOS PARA LA CONTRUCCION JANDRI S.A.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1711,14 +1711,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DEPODECON S.A.</t>
+          <t>COZZARELLI CONTRERAS FATIMA MERCEDES</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>179.1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
@@ -1771,14 +1771,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DIAZ CHAVEZ DIEGO FERNANDO</t>
+          <t>DEPODECON S.A.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0</v>
+        <v>179.1</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DISTRIBUIDORA Y SERVICIOS ELÉCTRICOS  ELEKTRICELL S.A.</t>
+          <t>DIAZ CHAVEZ DIEGO FERNANDO</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ELECTROKOLER S.A.</t>
+          <t>DISTRIBUIDORA Y SERVICIOS ELÉCTRICOS  ELEKTRICELL S.A.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FERRETERIA Y MADERAS S.A. MADEFER</t>
+          <t>ELECTROKOLER S.A.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>FLORES PARRA CLEIVER YOEL</t>
+          <t>FERRETERIA Y MADERAS S.A. MADEFER</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>GRANDA SANDOVAL JACKELINE ELIZABETH</t>
+          <t>FLORES PARRA CLEIVER YOEL</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
@@ -2102,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="n">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="M27" s="2" t="n">
-        <v>114.77</v>
+        <v>0</v>
       </c>
       <c r="N27" s="2" t="n">
         <v>0</v>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>GRATEROL CASTILLO STEFFANY PAOLA ROSDALY</t>
+          <t>GRANDA SANDOVAL JACKELINE ELIZABETH</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
@@ -2162,10 +2162,10 @@
         <v>0</v>
       </c>
       <c r="L28" s="2" t="n">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="M28" s="2" t="n">
-        <v>0</v>
+        <v>114.77</v>
       </c>
       <c r="N28" s="2" t="n">
         <v>0</v>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>GUILLEN PARRALES KATERINE MABEL</t>
+          <t>GRATEROL CASTILLO STEFFANY PAOLA ROSDALY</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>GUZMAN MAYORGA ROMINA SISNEY</t>
+          <t>GUILLEN PARRALES KATERINE MABEL</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>IMPORTADORA ORTEGA CIA. LTDA.</t>
+          <t>GUZMAN MAYORGA ROMINA SISNEY</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
+          <t>IMPORTADORA ORTEGA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
@@ -2390,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>843.72</v>
+        <v>0</v>
       </c>
       <c r="I32" s="2" t="n">
         <v>0</v>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
+          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>0</v>
+        <v>843.72</v>
       </c>
       <c r="I33" s="2" t="n">
         <v>0</v>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>JUAREZ FLORES JORGE WILLIAMS</t>
+          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LUI WONG ANGEL BOLIVAR</t>
+          <t>JUAREZ FLORES JORGE WILLIAMS</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MENA COSTA GUIDO LENNIN</t>
+          <t>LUI WONG ANGEL BOLIVAR</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MINUTOCORP S.A.</t>
+          <t>MENA COSTA GUIDO LENNIN</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
+          <t>MINUTOCORP S.A.</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MORALES GRACIELA ENITH</t>
+          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -2851,7 +2851,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
+          <t>MORALES GRACIELA ENITH</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
+          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -3185,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="2" t="n">
-        <v>94.56</v>
+        <v>0</v>
       </c>
       <c r="N45" s="2" t="n">
         <v>0</v>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -3245,7 +3245,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="2" t="n">
-        <v>0</v>
+        <v>94.56</v>
       </c>
       <c r="N46" s="2" t="n">
         <v>0</v>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -3691,7 +3691,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
@@ -3785,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="M55" s="2" t="n">
-        <v>48.91</v>
+        <v>0</v>
       </c>
       <c r="N55" s="2" t="n">
         <v>0</v>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C56" s="2" t="n">
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="2" t="n">
-        <v>4275.73</v>
+        <v>48.91</v>
       </c>
       <c r="N56" s="2" t="n">
         <v>0</v>
@@ -3871,137 +3871,197 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" s="2" t="n">
+        <v>4275.73</v>
+      </c>
+      <c r="N57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R57" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R57" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="C58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="D58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="E58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="F58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="G58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="H58" s="4" t="inlineStr">
-        <is>
-          <t>2 de 56</t>
-        </is>
-      </c>
-      <c r="I58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="J58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="K58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="L58" s="4" t="inlineStr">
-        <is>
-          <t>3 de 56</t>
-        </is>
-      </c>
-      <c r="M58" s="4" t="inlineStr">
-        <is>
-          <t>5 de 56</t>
-        </is>
-      </c>
-      <c r="N58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="O58" s="4" t="inlineStr">
-        <is>
-          <t>1 de 56</t>
-        </is>
-      </c>
-      <c r="P58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="Q58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
-        </is>
-      </c>
-      <c r="R58" s="4" t="inlineStr">
-        <is>
-          <t>0 de 56</t>
+      <c r="C58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
+        </is>
+      </c>
+      <c r="D59" s="4" t="inlineStr">
+        <is>
+          <t>1 de 57</t>
+        </is>
+      </c>
+      <c r="E59" s="4" t="inlineStr">
+        <is>
+          <t>1 de 57</t>
+        </is>
+      </c>
+      <c r="F59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
+        </is>
+      </c>
+      <c r="G59" s="4" t="inlineStr">
+        <is>
+          <t>1 de 57</t>
+        </is>
+      </c>
+      <c r="H59" s="4" t="inlineStr">
+        <is>
+          <t>2 de 57</t>
+        </is>
+      </c>
+      <c r="I59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
+        </is>
+      </c>
+      <c r="J59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
+        </is>
+      </c>
+      <c r="K59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
+        </is>
+      </c>
+      <c r="L59" s="4" t="inlineStr">
+        <is>
+          <t>3 de 57</t>
+        </is>
+      </c>
+      <c r="M59" s="4" t="inlineStr">
+        <is>
+          <t>5 de 57</t>
+        </is>
+      </c>
+      <c r="N59" s="4" t="inlineStr">
+        <is>
+          <t>1 de 57</t>
+        </is>
+      </c>
+      <c r="O59" s="4" t="inlineStr">
+        <is>
+          <t>1 de 57</t>
+        </is>
+      </c>
+      <c r="P59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
+        </is>
+      </c>
+      <c r="Q59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
+        </is>
+      </c>
+      <c r="R59" s="4" t="inlineStr">
+        <is>
+          <t>0 de 57</t>
         </is>
       </c>
     </row>
@@ -4016,7 +4076,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4132,7 +4192,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ALVAREZ SAAVEDRA EDWIN GEOVANNY</t>
+          <t>ALTAMIRANO VILLAVICENCIO JUAN ALEJANDRO</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -4148,7 +4208,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -4159,7 +4219,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ANGAMARCA CURIPONA WILMA</t>
+          <t>ALVAREZ SAAVEDRA EDWIN GEOVANNY</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -4175,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
@@ -4186,7 +4246,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ARIAS MEZA RONALD FABRICIO</t>
+          <t>ANGAMARCA CURIPONA WILMA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -4196,13 +4256,13 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>4990.88</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>2003.44</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -4213,7 +4273,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ARMIJOS SALINAS LUIS CLAUDIO</t>
+          <t>ARIAS MEZA RONALD FABRICIO</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -4223,13 +4283,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0</v>
+        <v>4990.88</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0</v>
+        <v>2003.44</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8">
@@ -4240,7 +4300,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ARREAGA DELGADO ITALO TEOBALDO</t>
+          <t>ARMIJOS SALINAS LUIS CLAUDIO</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -4267,7 +4327,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BADILLO VERGARA MARIELA MARIA</t>
+          <t>ARREAGA DELGADO ITALO TEOBALDO</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -4277,13 +4337,13 @@
         <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>2938.7</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -4294,23 +4354,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BORJA TORRES LETTY JANET</t>
+          <t>BADILLO VERGARA MARIELA MARIA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>18249.33</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>3793.28</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>24572.5</v>
+        <v>2938.7</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>2734.57</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>8000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="11">
@@ -4321,23 +4381,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BRIONES DIAZ HECTOR FERNANDO</t>
+          <t>BORJA TORRES LETTY JANET</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0</v>
+        <v>18249.33</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>3793.28</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0</v>
+        <v>24572.5</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>2734.57</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="12">
@@ -4348,23 +4408,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BUENAÑO VITERI MARJORIE LETICIA</t>
+          <t>BRIONES DIAZ HECTOR FERNANDO</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>1888.52</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>8385.370000000001</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>850.78</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -4375,23 +4435,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CALERO LOPEZ GISELLA JACKELINE</t>
+          <t>BUENAÑO VITERI MARJORIE LETICIA</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0</v>
+        <v>1888.52</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0</v>
+        <v>8385.370000000001</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>850.78</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="14">
@@ -4402,7 +4462,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CARREÑO SANCHEZ ITALO VICENTE</t>
+          <t>CALERO LOPEZ GISELLA JACKELINE</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -4429,7 +4489,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CASA FERRETERIA FONG S.A. FERREFONG</t>
+          <t>CARREÑO SANCHEZ ITALO VICENTE</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -4456,14 +4516,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CHASI PASTO ANGEL NOLBERTO</t>
+          <t>CASA FERRETERIA FONG S.A. FERREFONG</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>6711.78</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>9019.799999999999</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>0</v>
@@ -4472,7 +4532,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -4483,14 +4543,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>COMERCIALIZADORA &amp; CONSTRUCTORA ELECTRICA PALAU &amp; ORTIZ MEGA-ENERGYCORP SA</t>
+          <t>CHASI PASTO ANGEL NOLBERTO</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>6711.78</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>9019.799999999999</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
@@ -4499,7 +4559,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="18">
@@ -4510,7 +4570,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>COMERCIALIZADORA RAMIREZ GALVAN CIA. LTDA</t>
+          <t>COMERCIALIZADORA &amp; CONSTRUCTORA ELECTRICA PALAU &amp; ORTIZ MEGA-ENERGYCORP SA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -4537,7 +4597,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CONTRATISTAS ACABADOS PARA LA CONTRUCCION JANDRI S.A.</t>
+          <t>COMERCIALIZADORA RAMIREZ GALVAN CIA. LTDA</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -4553,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -4564,7 +4624,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>COZZARELLI CONTRERAS FATIMA MERCEDES</t>
+          <t>CONTRATISTAS ACABADOS PARA LA CONTRUCCION JANDRI S.A.</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -4580,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="21">
@@ -4591,7 +4651,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>DEPODECON S.A.</t>
+          <t>COZZARELLI CONTRERAS FATIMA MERCEDES</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -4604,7 +4664,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>179.1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>0</v>
@@ -4618,7 +4678,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>DIAZ CHAVEZ DIEGO FERNANDO</t>
+          <t>DEPODECON S.A.</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
@@ -4631,10 +4691,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0</v>
+        <v>179.1</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -4645,7 +4705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DISTRIBUIDORA Y SERVICIOS ELÉCTRICOS  ELEKTRICELL S.A.</t>
+          <t>DIAZ CHAVEZ DIEGO FERNANDO</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
@@ -4661,7 +4721,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="24">
@@ -4672,7 +4732,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ELECTROKOLER S.A.</t>
+          <t>DISTRIBUIDORA Y SERVICIOS ELÉCTRICOS  ELEKTRICELL S.A.</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
@@ -4699,7 +4759,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>FERRETERIA Y MADERAS S.A. MADEFER</t>
+          <t>ELECTROKOLER S.A.</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
@@ -4726,23 +4786,23 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>FLORES PARRA CLEIVER YOEL</t>
+          <t>FERRETERIA Y MADERAS S.A. MADEFER</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>8756.98</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>15779.69</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>1980.92</v>
+        <v>0</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -4753,23 +4813,23 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>GRANDA SANDOVAL JACKELINE ELIZABETH</t>
+          <t>FLORES PARRA CLEIVER YOEL</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>3865.18</v>
+        <v>8756.98</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>714.15</v>
+        <v>15779.69</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>1212.58</v>
+        <v>1980.92</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>261.77</v>
+        <v>0</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="28">
@@ -4780,23 +4840,23 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>GRATEROL CASTILLO STEFFANY PAOLA ROSDALY</t>
+          <t>GRANDA SANDOVAL JACKELINE ELIZABETH</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>0</v>
+        <v>3865.18</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>0</v>
+        <v>714.15</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>0</v>
+        <v>1212.58</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>0</v>
+        <v>261.77</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="29">
@@ -4807,23 +4867,23 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>GUILLEN PARRALES KATERINE MABEL</t>
+          <t>GRATEROL CASTILLO STEFFANY PAOLA ROSDALY</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>787.97</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>23.76</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>1670.44</v>
+        <v>0</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -4834,23 +4894,23 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>GUZMAN MAYORGA ROMINA SISNEY</t>
+          <t>GUILLEN PARRALES KATERINE MABEL</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0</v>
+        <v>787.97</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0</v>
+        <v>23.76</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0</v>
+        <v>1670.44</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="31">
@@ -4861,23 +4921,23 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>IMPORTADORA ORTEGA CIA. LTDA.</t>
+          <t>GUZMAN MAYORGA ROMINA SISNEY</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>4575.95</v>
+        <v>0</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>207.29</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32">
@@ -4888,23 +4948,23 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
+          <t>IMPORTADORA ORTEGA CIA. LTDA.</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0</v>
+        <v>4575.95</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0</v>
+        <v>207.29</v>
       </c>
       <c r="F32" s="2" t="n">
-        <v>843.72</v>
+        <v>0</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -4915,7 +4975,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
+          <t>INTERNEGOCIOS DE HIERRO S.A.</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
@@ -4928,10 +4988,10 @@
         <v>0</v>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0</v>
+        <v>843.72</v>
       </c>
       <c r="G33" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="34">
@@ -4942,17 +5002,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>JUAREZ FLORES JORGE WILLIAMS</t>
+          <t>ITURRALDE ROSALES FRANKLIN DAVID</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>869.73</v>
+        <v>0</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>1914.26</v>
+        <v>0</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0</v>
@@ -4969,17 +5029,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LUI WONG ANGEL BOLIVAR</t>
+          <t>JUAREZ FLORES JORGE WILLIAMS</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>0</v>
+        <v>869.73</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>0</v>
+        <v>1914.26</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>0</v>
@@ -4996,7 +5056,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MENA COSTA GUIDO LENNIN</t>
+          <t>LUI WONG ANGEL BOLIVAR</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
@@ -5023,7 +5083,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>MINUTOCORP S.A.</t>
+          <t>MENA COSTA GUIDO LENNIN</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
@@ -5036,7 +5096,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="n">
-        <v>68536.67999999999</v>
+        <v>0</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>0</v>
@@ -5050,7 +5110,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
+          <t>MINUTOCORP S.A.</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
@@ -5063,7 +5123,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="n">
-        <v>0</v>
+        <v>68536.67999999999</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>0</v>
@@ -5077,7 +5137,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MORALES GRACIELA ENITH</t>
+          <t>MONTAÑO JIMENEZ SANDRA GABRIELA</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
@@ -5104,14 +5164,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
+          <t>MORALES GRACIELA ENITH</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>86.40000000000001</v>
+        <v>0</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
@@ -5120,7 +5180,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -5131,14 +5191,14 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
+          <t>MUÑOZ FALCONES SERGIO BACILIO</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>0</v>
+        <v>86.40000000000001</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>0</v>
@@ -5147,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="42">
@@ -5158,7 +5218,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>ORTIZ GRANDA ANDREA DEL CISNE</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
@@ -5185,7 +5245,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -5212,23 +5272,23 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>1167.85</v>
+        <v>0</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>1053.12</v>
+        <v>0</v>
       </c>
       <c r="E44" s="2" t="n">
-        <v>2128.28</v>
+        <v>0</v>
       </c>
       <c r="F44" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G44" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -5239,23 +5299,23 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>737.72</v>
+        <v>1167.85</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>1696.97</v>
+        <v>1053.12</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>785.08</v>
+        <v>2128.28</v>
       </c>
       <c r="F45" s="2" t="n">
-        <v>94.56</v>
+        <v>0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>4500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="46">
@@ -5266,23 +5326,23 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>0</v>
+        <v>737.72</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>0</v>
+        <v>1696.97</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>0</v>
+        <v>785.08</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>0</v>
+        <v>94.56</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>0</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="47">
@@ -5293,7 +5353,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
@@ -5320,11 +5380,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>598.58</v>
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="n">
         <v>0</v>
@@ -5347,23 +5407,23 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>3470.45</v>
+        <v>598.58</v>
       </c>
       <c r="D49" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>2249.02</v>
+        <v>0</v>
       </c>
       <c r="F49" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G49" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -5374,23 +5434,23 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>0</v>
+        <v>3470.45</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>84.90000000000001</v>
+        <v>0</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>0</v>
+        <v>2249.02</v>
       </c>
       <c r="F50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="51">
@@ -5401,23 +5461,23 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>3819.46</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>1516.62</v>
+        <v>0</v>
       </c>
       <c r="F51" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>3500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -5428,23 +5488,23 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>0</v>
+        <v>3819.46</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>0</v>
+        <v>1516.62</v>
       </c>
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="53">
@@ -5455,7 +5515,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -5482,7 +5542,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -5509,23 +5569,23 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>48.91</v>
+        <v>0</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -5536,23 +5596,23 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C56" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E56" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F56" s="2" t="n">
-        <v>4275.73</v>
+        <v>48.91</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="57">
@@ -5563,39 +5623,66 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>4275.73</v>
+      </c>
+      <c r="G57" s="2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C57" s="2" t="n">
+      <c r="C58" s="2" t="n">
         <v>808.39</v>
       </c>
-      <c r="D57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" s="2" t="n">
+      <c r="D58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="58">
-      <c r="C58" s="6" t="n">
+    <row r="59">
+      <c r="C59" s="6" t="n">
         <v>50358.9</v>
       </c>
-      <c r="D58" s="6" t="n">
+      <c r="D59" s="6" t="n">
         <v>43293.1</v>
       </c>
-      <c r="E58" s="6" t="n">
+      <c r="E59" s="6" t="n">
         <v>64672.74</v>
       </c>
-      <c r="F58" s="6" t="n">
+      <c r="F59" s="6" t="n">
         <v>81432.43999999999</v>
       </c>
-      <c r="G58" s="6" t="n">
+      <c r="G59" s="6" t="n">
         <v>57000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-08-22 16:45:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="O28" s="2" t="n">
-        <v>0</v>
+        <v>1013.35</v>
       </c>
       <c r="P28" s="2" t="n">
         <v>0</v>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="O59" s="4" t="inlineStr">
         <is>
-          <t>1 de 57</t>
+          <t>2 de 57</t>
         </is>
       </c>
       <c r="P59" s="4" t="inlineStr">
@@ -4853,7 +4853,7 @@
         <v>1212.58</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>290.97</v>
+        <v>1304.32</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>2000</v>
@@ -5680,7 +5680,7 @@
         <v>64672.74</v>
       </c>
       <c r="F59" s="6" t="n">
-        <v>82832.7</v>
+        <v>83846.04999999999</v>
       </c>
       <c r="G59" s="6" t="n">
         <v>57000</v>
@@ -6144,13 +6144,13 @@
         <v>2300</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>2003.44</v>
+        <v>3016.79</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>296.5599999999999</v>
+        <v>-716.79</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>0.8710608695652174</v>
+        <v>1.311647826086956</v>
       </c>
     </row>
     <row r="19">
@@ -6163,13 +6163,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>14353.84</v>
+        <v>15367.19</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51001.26560036207</v>
+        <v>49987.91560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.219628441697759</v>
+        <v>0.235133733758589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-22 16:50:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="O51" s="2" t="n">
-        <v>0</v>
+        <v>2257.02</v>
       </c>
       <c r="P51" s="2" t="n">
         <v>0</v>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="O59" s="4" t="inlineStr">
         <is>
-          <t>2 de 57</t>
+          <t>3 de 57</t>
         </is>
       </c>
       <c r="P59" s="4" t="inlineStr">
@@ -5474,7 +5474,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="n">
-        <v>0</v>
+        <v>2257.02</v>
       </c>
       <c r="G51" s="2" t="n">
         <v>0</v>
@@ -5680,7 +5680,7 @@
         <v>64672.74</v>
       </c>
       <c r="F59" s="6" t="n">
-        <v>83846.04999999999</v>
+        <v>86103.06999999999</v>
       </c>
       <c r="G59" s="6" t="n">
         <v>57000</v>
@@ -6144,13 +6144,13 @@
         <v>2300</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>3016.79</v>
+        <v>5273.81</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>-716.79</v>
+        <v>-2973.81</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>1.311647826086956</v>
+        <v>2.292960869565217</v>
       </c>
     </row>
     <row r="19">
@@ -6163,13 +6163,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>15367.19</v>
+        <v>17624.21</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>49987.91560036207</v>
+        <v>47730.89560036208</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.235133733758589</v>
+        <v>0.2696684495893824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-28 16:50:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3965,7 +3965,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="2" t="n">
-        <v>1927.44</v>
+        <v>1329.51</v>
       </c>
       <c r="N58" s="2" t="n">
         <v>0</v>
@@ -5663,7 +5663,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="n">
-        <v>1927.44</v>
+        <v>1329.51</v>
       </c>
       <c r="G58" s="2" t="n">
         <v>1000</v>
@@ -5680,7 +5680,7 @@
         <v>64672.74</v>
       </c>
       <c r="F59" s="6" t="n">
-        <v>87291.62999999999</v>
+        <v>86693.7</v>
       </c>
       <c r="G59" s="6" t="n">
         <v>57000</v>
@@ -6096,13 +6096,13 @@
         <v>50390.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>6548.34</v>
+        <v>5950.41</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>43841.83</v>
+        <v>44439.75999999999</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1299527268909789</v>
+        <v>0.1180867220729757</v>
       </c>
     </row>
     <row r="17">
@@ -6163,13 +6163,13 @@
         <v>65355.10560036207</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>18812.77</v>
+        <v>18214.84</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46542.33560036208</v>
+        <v>47140.26560036207</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2878546339598567</v>
+        <v>0.2787056930392151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-01 17:15:06
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:R60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>PACHAR TAPIA ELIANA DE LOS ANGELES</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
@@ -3211,7 +3211,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
@@ -3271,7 +3271,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
@@ -3631,7 +3631,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
@@ -3691,7 +3691,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C56" s="2" t="n">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C57" s="2" t="n">
@@ -3931,137 +3931,197 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R58" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="C59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="D59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="E59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="F59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="G59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="H59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="I59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="J59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="K59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="L59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="M59" s="4" t="inlineStr">
-        <is>
-          <t>1 de 57</t>
-        </is>
-      </c>
-      <c r="N59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="O59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="P59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="Q59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
-        </is>
-      </c>
-      <c r="R59" s="4" t="inlineStr">
-        <is>
-          <t>0 de 57</t>
+      <c r="C59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R59" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="D60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="H60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="I60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="J60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="K60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="L60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="M60" s="4" t="inlineStr">
+        <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="N60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="O60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="P60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="Q60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="R60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
         </is>
       </c>
     </row>
@@ -4076,7 +4136,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5245,7 +5305,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PUCO TOAPANTA MARCO ANTONIO</t>
+          <t>PACHAR TAPIA ELIANA DE LOS ANGELES</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
@@ -5272,7 +5332,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
+          <t>PUCO TOAPANTA MARCO ANTONIO</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
@@ -5299,23 +5359,23 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
+          <t>QUIÑONEZ LEON MARIA PURIFICACION</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>1053.12</v>
+        <v>0</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>2128.28</v>
+        <v>0</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>91.58</v>
+        <v>0</v>
       </c>
       <c r="F45" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -5326,23 +5386,23 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>RUALES SARAGURO JIMMY JAVIER</t>
+          <t>ROBLES CAMPOVERDE TANIA CRISTINA</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>1696.97</v>
+        <v>1053.12</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>785.08</v>
+        <v>2128.28</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>2174</v>
+        <v>91.58</v>
       </c>
       <c r="F46" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>4500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="47">
@@ -5353,23 +5413,23 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SANCHEZ BAJANA FRAK XAVIER</t>
+          <t>RUALES SARAGURO JIMMY JAVIER</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>0</v>
+        <v>1696.97</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>0</v>
+        <v>785.08</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>0</v>
+        <v>2174</v>
       </c>
       <c r="F47" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>0</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="48">
@@ -5380,7 +5440,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SANCHEZ CORREA WILSON SERGIO</t>
+          <t>SANCHEZ BAJANA FRAK XAVIER</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
@@ -5407,7 +5467,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
+          <t>SANCHEZ CORREA WILSON SERGIO</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
@@ -5434,23 +5494,23 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
+          <t>SANDOVAL GONZALEZ LAUTARO MARCELO</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>2249.02</v>
+        <v>0</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>64.45999999999999</v>
+        <v>0</v>
       </c>
       <c r="F50" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G50" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -5461,23 +5521,23 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
+          <t>SANDOVAL GONZALEZ NILO GUILLERMO</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>84.90000000000001</v>
+        <v>0</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>0</v>
+        <v>2249.02</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>2257.02</v>
+        <v>64.45999999999999</v>
       </c>
       <c r="F51" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="52">
@@ -5488,23 +5548,23 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
+          <t>SARITAMA HERRERA MARIA ELIZABETH</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
-        <v>3819.46</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>1516.62</v>
+        <v>0</v>
       </c>
       <c r="E52" s="2" t="n">
-        <v>0</v>
+        <v>2257.02</v>
       </c>
       <c r="F52" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>3500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -5515,14 +5575,14 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
+          <t>SIMANCAS AGUILAR HONORIO ANTONIO</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>0</v>
+        <v>3819.46</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>0</v>
+        <v>1516.62</v>
       </c>
       <c r="E53" s="2" t="n">
         <v>0</v>
@@ -5531,7 +5591,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="54">
@@ -5542,7 +5602,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SOPLIN MENDOZA TABITA</t>
+          <t>SOCIEDAD CIVIL Y COMERCIAL GRUPO MOLINA PROAÑO</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
@@ -5569,7 +5629,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
+          <t>SOPLIN MENDOZA TABITA</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
@@ -5596,23 +5656,23 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
+          <t>SORIA AVELLAN RAFAEL HUMBERTO</t>
         </is>
       </c>
       <c r="C56" s="2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D56" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>48.91</v>
+        <v>0</v>
       </c>
       <c r="F56" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -5623,23 +5683,23 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>VERA CABRERA JORGE ENRIQUE</t>
+          <t>VEINTIMILLA JARAMILLO HERMANOS VJHNOS S.A.S.</t>
         </is>
       </c>
       <c r="C57" s="2" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D57" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>4275.73</v>
+        <v>48.91</v>
       </c>
       <c r="F57" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>5000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="58">
@@ -5650,39 +5710,66 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>VERA CABRERA JORGE ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>4275.73</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>VIVANCO MALDONADO SILVANA MARILY</t>
         </is>
       </c>
-      <c r="C58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="n">
+      <c r="C59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="n">
         <v>1329.51</v>
       </c>
-      <c r="F58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" s="2" t="n">
+      <c r="F59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="59">
-      <c r="C59" s="6" t="n">
+    <row r="60">
+      <c r="C60" s="6" t="n">
         <v>43293.1</v>
       </c>
-      <c r="D59" s="6" t="n">
+      <c r="D60" s="6" t="n">
         <v>64672.74</v>
       </c>
-      <c r="E59" s="6" t="n">
+      <c r="E60" s="6" t="n">
         <v>88332.23999999999</v>
       </c>
-      <c r="F59" s="6" t="n">
+      <c r="F60" s="6" t="n">
         <v>131.54</v>
       </c>
-      <c r="G59" s="6" t="n">
+      <c r="G60" s="6" t="n">
         <v>57000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-09-09 16:55:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0</v>
+        <v>1339.12</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0</v>
+        <v>545.6</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>0</v>
@@ -4056,37 +4056,37 @@
       </c>
       <c r="E60" s="4" t="inlineStr">
         <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="F60" s="4" t="inlineStr">
+      <c r="G60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="G60" s="4" t="inlineStr">
+      <c r="H60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="H60" s="4" t="inlineStr">
+      <c r="I60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="I60" s="4" t="inlineStr">
+      <c r="J60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="J60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
       <c r="K60" s="4" t="inlineStr">
         <is>
-          <t>0 de 58</t>
+          <t>1 de 58</t>
         </is>
       </c>
       <c r="L60" s="4" t="inlineStr">
@@ -4454,7 +4454,7 @@
         <v>2734.57</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>1884.72</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>5000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>958.98</v>
+        <v>2843.7</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -5795,8 +5795,8 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -5895,13 +5895,13 @@
         <v>1304.0286065816</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>1339.12</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>1304.0286065816</v>
+        <v>-35.0913934184</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>1.026909987435313</v>
       </c>
     </row>
     <row r="5">
@@ -6039,13 +6039,13 @@
         <v>388.107983534392</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>545.6</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>388.107983534392</v>
+        <v>-157.492016465608</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0</v>
+        <v>1.405794323093722</v>
       </c>
     </row>
     <row r="11">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>958.98</v>
+        <v>2843.7</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>49524.7870510252</v>
+        <v>47640.0670510252</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.0189958090692942</v>
+        <v>0.05632899773754604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-09 17:00:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="2" t="n">
-        <v>0</v>
+        <v>2922.66</v>
       </c>
       <c r="O16" s="2" t="n">
         <v>0</v>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="N60" s="4" t="inlineStr">
         <is>
-          <t>0 de 58</t>
+          <t>1 de 58</t>
         </is>
       </c>
       <c r="O60" s="4" t="inlineStr">
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>2922.66</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>2500</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>2843.7</v>
+        <v>5766.36</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -6111,13 +6111,13 @@
         <v>1332.52398144409</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>0</v>
+        <v>2922.66</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>1332.52398144409</v>
+        <v>-1590.13601855591</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>0</v>
+        <v>2.193326379636815</v>
       </c>
     </row>
     <row r="14">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>2843.7</v>
+        <v>5766.360000000001</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>47640.0670510252</v>
+        <v>44717.40705102521</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.05632899773754604</v>
+        <v>0.1142220625923536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-10 09:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>545.6</v>
+        <v>600.16</v>
       </c>
       <c r="L11" s="2" t="n">
         <v>0</v>
@@ -4454,7 +4454,7 @@
         <v>2734.57</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1884.72</v>
+        <v>1939.28</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>5000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>5766.36</v>
+        <v>5820.92</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -5796,7 +5796,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -6039,13 +6039,13 @@
         <v>388.107983534392</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>545.6</v>
+        <v>600.16</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>-157.492016465608</v>
+        <v>-212.0520164656079</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>1.405794323093722</v>
+        <v>1.546373755403094</v>
       </c>
     </row>
     <row r="11">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>5766.360000000001</v>
+        <v>5820.92</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>44717.40705102521</v>
+        <v>44662.84705102521</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.1142220625923536</v>
+        <v>0.1153028060310288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-11 09:20:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>950.4</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
@@ -1490,10 +1490,10 @@
         <v>0</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>0</v>
+        <v>559.6799999999999</v>
       </c>
       <c r="J17" s="2" t="n">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>0</v>
+        <v>3758.1</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>0</v>
@@ -4051,52 +4051,52 @@
       </c>
       <c r="D60" s="4" t="inlineStr">
         <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="E60" s="4" t="inlineStr">
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="H60" s="4" t="inlineStr">
         <is>
           <t>1 de 58</t>
         </is>
       </c>
-      <c r="F60" s="4" t="inlineStr">
+      <c r="I60" s="4" t="inlineStr">
+        <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="J60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="G60" s="4" t="inlineStr">
+      <c r="K60" s="4" t="inlineStr">
+        <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="L60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="H60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="I60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="J60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="K60" s="4" t="inlineStr">
-        <is>
-          <t>1 de 58</t>
-        </is>
-      </c>
-      <c r="L60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>2 de 58</t>
+          <t>3 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -4616,7 +4616,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0</v>
+        <v>6456.18</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>3000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>5865.27</v>
+        <v>12321.45</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -5797,7 +5797,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5871,13 +5871,13 @@
         <v>5504.61890386263</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>950.4</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>5504.61890386263</v>
+        <v>4554.21890386263</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.1726550042062126</v>
       </c>
     </row>
     <row r="4">
@@ -5943,13 +5943,13 @@
         <v>849.84419682004</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>849.84419682004</v>
+        <v>-338.15580317996</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>1.397903291503639</v>
       </c>
     </row>
     <row r="7">
@@ -5967,13 +5967,13 @@
         <v>709.368813030059</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>559.6799999999999</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>709.368813030059</v>
+        <v>149.688813030059</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>0.7889830927431595</v>
       </c>
     </row>
     <row r="8">
@@ -6087,13 +6087,13 @@
         <v>32404.8</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>298.31</v>
+        <v>4056.41</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>32106.49</v>
+        <v>28348.39</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.009205734952846493</v>
+        <v>0.1251792944255172</v>
       </c>
     </row>
     <row r="13">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>5865.27</v>
+        <v>12321.45</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>44618.49705102521</v>
+        <v>38162.31705102521</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.116181306241902</v>
+        <v>0.2440675630950124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-11 16:00:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0</v>
+        <v>1054.31</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>3 de 58</t>
+          <t>4 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -4211,7 +4211,7 @@
         <v>1603.18</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0</v>
+        <v>1054.31</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>3000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>12321.45</v>
+        <v>13375.76</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -6087,13 +6087,13 @@
         <v>32404.8</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>4056.41</v>
+        <v>5110.72</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>28348.39</v>
+        <v>27294.08</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.1251792944255172</v>
+        <v>0.1577149064336148</v>
       </c>
     </row>
     <row r="13">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>12321.45</v>
+        <v>13375.76</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>38162.31705102521</v>
+        <v>37108.00705102521</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.2440675630950124</v>
+        <v>0.2649517019298656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 16:50:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0</v>
+        <v>633.12</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0</v>
+        <v>1037.85</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>0</v>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>5802.23</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -2930,10 +2930,10 @@
         <v>0</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>0</v>
+        <v>1010.7</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>0</v>
+        <v>26.1</v>
       </c>
       <c r="J41" s="2" t="n">
         <v>0</v>
@@ -4056,47 +4056,47 @@
       </c>
       <c r="E60" s="4" t="inlineStr">
         <is>
+          <t>2 de 58</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="H60" s="4" t="inlineStr">
+        <is>
+          <t>3 de 58</t>
+        </is>
+      </c>
+      <c r="I60" s="4" t="inlineStr">
+        <is>
+          <t>2 de 58</t>
+        </is>
+      </c>
+      <c r="J60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="K60" s="4" t="inlineStr">
+        <is>
           <t>1 de 58</t>
         </is>
       </c>
-      <c r="F60" s="4" t="inlineStr">
+      <c r="L60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="G60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="H60" s="4" t="inlineStr">
-        <is>
-          <t>1 de 58</t>
-        </is>
-      </c>
-      <c r="I60" s="4" t="inlineStr">
-        <is>
-          <t>1 de 58</t>
-        </is>
-      </c>
-      <c r="J60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="K60" s="4" t="inlineStr">
-        <is>
-          <t>1 de 58</t>
-        </is>
-      </c>
-      <c r="L60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>4 de 58</t>
+          <t>5 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -4427,7 +4427,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>1670.97</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>2000</v>
@@ -4508,7 +4508,7 @@
         <v>850.78</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>5802.23</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>2000</v>
@@ -5264,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="n">
-        <v>0</v>
+        <v>1036.8</v>
       </c>
       <c r="G41" s="2" t="n">
         <v>1000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>13375.76</v>
+        <v>21885.76</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -5795,7 +5795,7 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
@@ -5895,13 +5895,13 @@
         <v>1304.0286065816</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>1339.12</v>
+        <v>1972.24</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>-35.0913934184</v>
+        <v>-668.2113934184001</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>1.026909987435313</v>
+        <v>1.512420808903924</v>
       </c>
     </row>
     <row r="5">
@@ -5943,13 +5943,13 @@
         <v>849.84419682004</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>1188</v>
+        <v>3236.55</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>-338.15580317996</v>
+        <v>-2386.70580317996</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>1.397903291503639</v>
+        <v>3.808403954643183</v>
       </c>
     </row>
     <row r="7">
@@ -5967,13 +5967,13 @@
         <v>709.368813030059</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>559.6799999999999</v>
+        <v>585.78</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>149.688813030059</v>
+        <v>123.588813030059</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.7889830927431595</v>
+        <v>0.8257763651856203</v>
       </c>
     </row>
     <row r="8">
@@ -6087,13 +6087,13 @@
         <v>32404.8</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>5110.72</v>
+        <v>10912.95</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>27294.08</v>
+        <v>21491.85</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.1577149064336148</v>
+        <v>0.3367695526588654</v>
       </c>
     </row>
     <row r="13">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>13375.76</v>
+        <v>21885.76</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>37108.00705102521</v>
+        <v>28598.0070510252</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.2649517019298656</v>
+        <v>0.4335207390106114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-22 16:10:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3245,7 +3245,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="2" t="n">
-        <v>0</v>
+        <v>2169.37</v>
       </c>
       <c r="N46" s="2" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>7 de 58</t>
+          <t>8 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -5399,7 +5399,7 @@
         <v>91.58</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>0</v>
+        <v>2169.37</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>2000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>30825.64</v>
+        <v>32995.01</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -6087,13 +6087,13 @@
         <v>32404.8</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>18867.86</v>
+        <v>21037.23</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>13536.94</v>
+        <v>11367.57</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.5822550980101714</v>
+        <v>0.6492010442897349</v>
       </c>
     </row>
     <row r="13">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>31064.46</v>
+        <v>33233.83</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>19419.3070510252</v>
+        <v>17249.9370510252</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.615335618053272</v>
+        <v>0.6583072528325737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-22 16:15:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>0</v>
+        <v>929.66</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>0</v>
@@ -3242,7 +3242,7 @@
         <v>0</v>
       </c>
       <c r="L46" s="2" t="n">
-        <v>0</v>
+        <v>293.99</v>
       </c>
       <c r="M46" s="2" t="n">
         <v>2169.37</v>
@@ -4051,39 +4051,39 @@
       </c>
       <c r="D60" s="4" t="inlineStr">
         <is>
+          <t>3 de 58</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>3 de 58</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="H60" s="4" t="inlineStr">
+        <is>
+          <t>3 de 58</t>
+        </is>
+      </c>
+      <c r="I60" s="4" t="inlineStr">
+        <is>
           <t>2 de 58</t>
         </is>
       </c>
-      <c r="E60" s="4" t="inlineStr">
-        <is>
-          <t>3 de 58</t>
-        </is>
-      </c>
-      <c r="F60" s="4" t="inlineStr">
+      <c r="J60" s="4" t="inlineStr">
         <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="G60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="H60" s="4" t="inlineStr">
-        <is>
-          <t>3 de 58</t>
-        </is>
-      </c>
-      <c r="I60" s="4" t="inlineStr">
-        <is>
-          <t>2 de 58</t>
-        </is>
-      </c>
-      <c r="J60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
       <c r="K60" s="4" t="inlineStr">
         <is>
           <t>1 de 58</t>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="L60" s="4" t="inlineStr">
         <is>
-          <t>0 de 58</t>
+          <t>1 de 58</t>
         </is>
       </c>
       <c r="M60" s="4" t="inlineStr">
@@ -5399,7 +5399,7 @@
         <v>91.58</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>2169.37</v>
+        <v>3393.02</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>2000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>32995.01</v>
+        <v>34218.66</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -5871,13 +5871,13 @@
         <v>5504.61890386263</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1866.24</v>
+        <v>2795.9</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>3638.37890386263</v>
+        <v>2708.71890386263</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.3390316446231085</v>
+        <v>0.5079189038932554</v>
       </c>
     </row>
     <row r="4">
@@ -6063,13 +6063,13 @@
         <v>3506.66949822329</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>238.82</v>
+        <v>532.8099999999999</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>3267.84949822329</v>
+        <v>2973.85949822329</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0.0681045077447424</v>
+        <v>0.1519418925193711</v>
       </c>
     </row>
     <row r="12">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>33233.83</v>
+        <v>34457.48</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>17249.9370510252</v>
+        <v>16026.2870510252</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.6583072528325737</v>
+        <v>0.6825457372302064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-22 16:20:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>0</v>
+        <v>288</v>
       </c>
       <c r="J53" s="2" t="n">
         <v>0</v>
@@ -3662,10 +3662,10 @@
         <v>0</v>
       </c>
       <c r="L53" s="2" t="n">
-        <v>0</v>
+        <v>537.34</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>0</v>
+        <v>1842.21</v>
       </c>
       <c r="N53" s="2" t="n">
         <v>0</v>
@@ -4076,27 +4076,27 @@
       </c>
       <c r="I60" s="4" t="inlineStr">
         <is>
+          <t>3 de 58</t>
+        </is>
+      </c>
+      <c r="J60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="K60" s="4" t="inlineStr">
+        <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="L60" s="4" t="inlineStr">
+        <is>
           <t>2 de 58</t>
         </is>
       </c>
-      <c r="J60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="K60" s="4" t="inlineStr">
-        <is>
-          <t>1 de 58</t>
-        </is>
-      </c>
-      <c r="L60" s="4" t="inlineStr">
-        <is>
-          <t>1 de 58</t>
-        </is>
-      </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>8 de 58</t>
+          <t>9 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -5588,7 +5588,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>0</v>
+        <v>2667.55</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>2500</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>34218.66</v>
+        <v>36886.21</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -5967,13 +5967,13 @@
         <v>709.368813030059</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>585.78</v>
+        <v>873.78</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>123.588813030059</v>
+        <v>-164.411186969941</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.8257763651856203</v>
+        <v>1.231771095585188</v>
       </c>
     </row>
     <row r="8">
@@ -6063,13 +6063,13 @@
         <v>3506.66949822329</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>532.8099999999999</v>
+        <v>1070.15</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2973.85949822329</v>
+        <v>2436.51949822329</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0.1519418925193711</v>
+        <v>0.3051756090906795</v>
       </c>
     </row>
     <row r="12">
@@ -6087,13 +6087,13 @@
         <v>32404.8</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>21037.23</v>
+        <v>22879.44</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>11367.57</v>
+        <v>9525.360000000001</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.6492010442897349</v>
+        <v>0.7060509554140127</v>
       </c>
     </row>
     <row r="13">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>34457.48</v>
+        <v>37125.02999999999</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>16026.2870510252</v>
+        <v>13358.73705102521</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.6825457372302064</v>
+        <v>0.7353854945586132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-26 16:40:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3305,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="2" t="n">
-        <v>2719.98</v>
+        <v>2785.75</v>
       </c>
       <c r="N47" s="2" t="n">
         <v>0</v>
@@ -5426,7 +5426,7 @@
         <v>2174</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>2719.98</v>
+        <v>2785.75</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>3000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>69656.06</v>
+        <v>69721.83</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -6087,13 +6087,13 @@
         <v>32404.8</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>55050.37</v>
+        <v>55116.14</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-22645.57</v>
+        <v>-22711.34</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>1.698833814743495</v>
+        <v>1.70086345232805</v>
       </c>
     </row>
     <row r="13">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>69822.86000000002</v>
+        <v>69888.63</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-19339.09294897479</v>
+        <v>-19404.86294897479</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>1.383075473140273</v>
+        <v>1.384378268154233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-29 09:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>30512.6</v>
+        <v>30271.32</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -4454,7 +4454,7 @@
         <v>2734.57</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>32451.88</v>
+        <v>32210.6</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>5000</v>
@@ -5767,7 +5767,7 @@
         <v>88332.23999999999</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>69721.83</v>
+        <v>69480.55</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>46000</v>
@@ -6087,13 +6087,13 @@
         <v>32404.8</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>55116.14</v>
+        <v>54874.86</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-22711.34</v>
+        <v>-22470.06</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>1.70086345232805</v>
+        <v>1.69341764183084</v>
       </c>
     </row>
     <row r="13">
@@ -6154,13 +6154,13 @@
         <v>50483.7670510252</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>69888.63</v>
+        <v>69647.35000000001</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>-19404.86294897479</v>
+        <v>-19163.5829489748</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>1.384378268154233</v>
+        <v>1.379598910073523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-07 10:30:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2885,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="2" t="n">
-        <v>0</v>
+        <v>829.4400000000001</v>
       </c>
       <c r="N40" s="2" t="n">
         <v>0</v>
@@ -3665,7 +3665,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>0</v>
+        <v>6635.52</v>
       </c>
       <c r="N53" s="2" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>0 de 58</t>
+          <t>2 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -5237,7 +5237,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="n">
-        <v>0</v>
+        <v>829.4400000000001</v>
       </c>
       <c r="G40" s="2" t="n">
         <v>0</v>
@@ -5588,7 +5588,7 @@
         <v>2667.55</v>
       </c>
       <c r="F53" s="2" t="n">
-        <v>0</v>
+        <v>6635.52</v>
       </c>
       <c r="G53" s="2" t="n">
         <v>0</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>955.0000000000001</v>
+        <v>8419.960000000001</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>0</v>
@@ -6087,13 +6087,13 @@
         <v>38542.25</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0</v>
+        <v>7464.96</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>38542.25</v>
+        <v>31077.29</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0</v>
+        <v>0.193682517237577</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>955</v>
+        <v>8419.959999999999</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>53528.76774946896</v>
+        <v>46063.80774946896</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.01752815635642798</v>
+        <v>0.1545407072197584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-07 12:30:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -4214,7 +4214,7 @@
         <v>1185.15</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3">
@@ -4241,7 +4241,7 @@
         <v>-230.15</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="4">
@@ -4349,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8">
@@ -4430,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="11">
@@ -4457,7 +4457,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="12">
@@ -4511,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="14">
@@ -4592,7 +4592,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17">
@@ -4619,7 +4619,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="18">
@@ -4700,7 +4700,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="21">
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="2" t="n">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="28">
@@ -4916,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="29">
@@ -4970,7 +4970,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31">
@@ -4997,7 +4997,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="2" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="32">
@@ -5267,7 +5267,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="42">
@@ -5402,7 +5402,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="47">
@@ -5429,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="48">
@@ -5591,7 +5591,7 @@
         <v>6635.52</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>0</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="54">
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="58">
@@ -5726,7 +5726,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="59">
@@ -5753,7 +5753,7 @@
         <v>0</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="60">
@@ -5770,7 +5770,7 @@
         <v>8419.960000000001</v>
       </c>
       <c r="G60" s="6" t="n">
-        <v>0</v>
+        <v>52000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-13 10:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3965,7 +3965,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="2" t="n">
-        <v>0</v>
+        <v>1115.07</v>
       </c>
       <c r="N58" s="2" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>3 de 58</t>
+          <t>4 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -5723,7 +5723,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="n">
-        <v>0</v>
+        <v>1115.07</v>
       </c>
       <c r="G58" s="2" t="n">
         <v>2000</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>8763.730000000001</v>
+        <v>9878.800000000001</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -6087,13 +6087,13 @@
         <v>38542.25</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>7808.73</v>
+        <v>8923.799999999999</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>30733.52</v>
+        <v>29618.45</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.2026018200805609</v>
+        <v>0.2315329281502766</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>8763.73</v>
+        <v>9878.799999999999</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>45720.03774946896</v>
+        <v>44604.96774946896</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.1608502928853597</v>
+        <v>0.1813163884962102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-13 15:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -665,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0</v>
+        <v>3284.43</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>4 de 58</t>
+          <t>5 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -4238,7 +4238,7 @@
         <v>1672.61</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>-230.15</v>
+        <v>3054.28</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>2500</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>9878.800000000001</v>
+        <v>13163.23</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -5795,7 +5795,7 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -6087,13 +6087,13 @@
         <v>38542.25</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>8923.799999999999</v>
+        <v>12208.23</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>29618.45</v>
+        <v>26334.02</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.2315329281502766</v>
+        <v>0.3167492816324942</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>9878.799999999999</v>
+        <v>13163.23</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>44604.96774946896</v>
+        <v>41320.53774946896</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.1813163884962102</v>
+        <v>0.2415991137126947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-14 15:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -605,7 +605,7 @@
         <v>790.78</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0</v>
+        <v>-70.28</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
@@ -4211,7 +4211,7 @@
         <v>2774.22</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1185.15</v>
+        <v>1114.87</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>2000</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>13163.23</v>
+        <v>13092.95</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -6087,13 +6087,13 @@
         <v>38542.25</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>12208.23</v>
+        <v>12137.95</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>26334.02</v>
+        <v>26404.3</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.3167492816324942</v>
+        <v>0.3149258281496281</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>13163.23</v>
+        <v>13092.95</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>41320.53774946896</v>
+        <v>41390.81774946896</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.2415991137126947</v>
+        <v>0.240309188237585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-16 16:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3305,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="2" t="n">
-        <v>1356</v>
+        <v>1743.18</v>
       </c>
       <c r="N47" s="2" t="n">
         <v>0</v>
@@ -5426,7 +5426,7 @@
         <v>2785.75</v>
       </c>
       <c r="F47" s="2" t="n">
-        <v>1356</v>
+        <v>1743.18</v>
       </c>
       <c r="G47" s="2" t="n">
         <v>3500</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>20298.42</v>
+        <v>20685.6</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -5795,7 +5795,7 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -6087,13 +6087,13 @@
         <v>38542.25</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>15998.3</v>
+        <v>16385.48</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>22543.95</v>
+        <v>22156.77</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.415084744663324</v>
+        <v>0.4251303439731723</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>20298.42</v>
+        <v>20685.6</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>34185.34774946896</v>
+        <v>33798.16774946896</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.3725590361763819</v>
+        <v>0.3796653729073576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-22 12:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>0</v>
+        <v>1068.48</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>0</v>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="D60" s="4" t="inlineStr">
         <is>
-          <t>1 de 58</t>
+          <t>2 de 58</t>
         </is>
       </c>
       <c r="E60" s="4" t="inlineStr">
@@ -5399,7 +5399,7 @@
         <v>3393.02</v>
       </c>
       <c r="F46" s="2" t="n">
-        <v>0</v>
+        <v>1068.48</v>
       </c>
       <c r="G46" s="2" t="n">
         <v>2000</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>23825.67</v>
+        <v>24894.15</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -5871,13 +5871,13 @@
         <v>5504.61890386263</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>177.06</v>
+        <v>1245.54</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>5327.558903862629</v>
+        <v>4259.07890386263</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.03216571448311449</v>
+        <v>0.2262717949694929</v>
       </c>
     </row>
     <row r="4">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>23825.67</v>
+        <v>24894.15</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>30658.09774946896</v>
+        <v>29589.61774946896</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.4372985016300056</v>
+        <v>0.4569094801679283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-24 13:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>2550.21</v>
+        <v>3241.38</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>0</v>
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="2" t="n">
-        <v>0</v>
+        <v>1782.27</v>
       </c>
       <c r="Q17" s="2" t="n">
         <v>0</v>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="P60" s="4" t="inlineStr">
         <is>
-          <t>1 de 58</t>
+          <t>2 de 58</t>
         </is>
       </c>
       <c r="Q60" s="4" t="inlineStr">
@@ -4616,7 +4616,7 @@
         <v>6456.18</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>2550.21</v>
+        <v>5023.65</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>3500</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>27444.36</v>
+        <v>29917.8</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -5991,13 +5991,13 @@
         <v>516.121873547834</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>1445.41</v>
+        <v>3227.68</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-929.2881264521661</v>
+        <v>-2711.558126452166</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>2.800520718225363</v>
+        <v>6.253716739057873</v>
       </c>
     </row>
     <row r="9">
@@ -6087,13 +6087,13 @@
         <v>38542.25</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>21631.02</v>
+        <v>22322.19</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>16911.23</v>
+        <v>16220.06</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.5612287814022274</v>
+        <v>0.5791615694465164</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>27444.36</v>
+        <v>29917.8</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>27039.40774946896</v>
+        <v>24565.96774946896</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.5037162651121442</v>
+        <v>0.5491140065343884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-28 17:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>10631.16</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>8 de 58</t>
+          <t>9 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -4454,7 +4454,7 @@
         <v>31952.93</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1591.79</v>
+        <v>12222.95</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>11000</v>
@@ -5767,7 +5767,7 @@
         <v>69222.88</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>35579.06</v>
+        <v>46210.22</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -6087,13 +6087,13 @@
         <v>38542.25</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>27435.76</v>
+        <v>38066.92</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>11106.49</v>
+        <v>475.3300000000017</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.7118359722123124</v>
+        <v>0.987667300170592</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>54483.76774946896</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>35579.06</v>
+        <v>46210.22</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>18904.70774946896</v>
+        <v>8273.547749468966</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.653021284497102</v>
+        <v>0.8481465564659008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-13 08:30:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>1115.09</v>
+        <v>1097.67</v>
       </c>
       <c r="N2" s="2" t="n">
         <v>0</v>
@@ -1142,10 +1142,10 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0</v>
+        <v>3036.24</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>7195.12</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -2258,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0</v>
+        <v>457.92</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0</v>
@@ -4051,52 +4051,52 @@
       </c>
       <c r="D60" s="4" t="inlineStr">
         <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="inlineStr">
+        <is>
+          <t>1 de 58</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
           <t>0 de 58</t>
         </is>
       </c>
-      <c r="E60" s="4" t="inlineStr">
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="H60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="I60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="J60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="K60" s="4" t="inlineStr">
+        <is>
+          <t>0 de 58</t>
+        </is>
+      </c>
+      <c r="L60" s="4" t="inlineStr">
         <is>
           <t>1 de 58</t>
         </is>
       </c>
-      <c r="F60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="G60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="H60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="I60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="J60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="K60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
-      <c r="L60" s="4" t="inlineStr">
-        <is>
-          <t>0 de 58</t>
-        </is>
-      </c>
       <c r="M60" s="4" t="inlineStr">
         <is>
-          <t>3 de 58</t>
+          <t>4 de 58</t>
         </is>
       </c>
       <c r="N60" s="4" t="inlineStr">
@@ -4211,7 +4211,7 @@
         <v>1114.87</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>1115.09</v>
+        <v>1097.67</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>2000</v>
@@ -4454,7 +4454,7 @@
         <v>12084.08</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>2172.1</v>
+        <v>12403.46</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>11000</v>
@@ -4967,7 +4967,7 @@
         <v>278.41</v>
       </c>
       <c r="F30" s="2" t="n">
-        <v>0</v>
+        <v>457.92</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>500</v>
@@ -5767,7 +5767,7 @@
         <v>54885.7</v>
       </c>
       <c r="F60" s="6" t="n">
-        <v>8823</v>
+        <v>19494.86</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>52000</v>
@@ -5795,7 +5795,7 @@
     <col width="26" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -5871,13 +5871,13 @@
         <v>1867.69</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>457.92</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>1867.69</v>
+        <v>1409.77</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.2451798746044579</v>
       </c>
     </row>
     <row r="4">
@@ -6063,13 +6063,13 @@
         <v>1440.92</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>3036.24</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>1440.92</v>
+        <v>-1595.32</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0</v>
+        <v>2.107153762873719</v>
       </c>
     </row>
     <row r="12">
@@ -6087,13 +6087,13 @@
         <v>48041</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>6621.41</v>
+        <v>13799.11</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>41419.59</v>
+        <v>34241.89</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.1378283133157095</v>
+        <v>0.2872361108220062</v>
       </c>
     </row>
     <row r="13">
@@ -6130,13 +6130,13 @@
         <v>57887.35196497848</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>8823</v>
+        <v>19494.86</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>49064.35196497847</v>
+        <v>38392.49196497848</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.1524167145413365</v>
+        <v>0.3367723576610359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-18 13:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -6015,10 +6015,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0</v>
+        <v>68536.67999999999</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0</v>
+        <v>-68536.67999999999</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
@@ -6130,13 +6130,13 @@
         <v>57887.35196497848</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>34097.58</v>
+        <v>102634.26</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>23789.77196497848</v>
+        <v>-44746.9080350215</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.5890333353066287</v>
+        <v>1.772999740290299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-27 08:30:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -6039,13 +6039,13 @@
         <v>388.107983534392</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>1425.24</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>388.107983534392</v>
+        <v>-1037.132016465608</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0</v>
+        <v>3.672276944732581</v>
       </c>
     </row>
     <row r="11">
@@ -6063,13 +6063,13 @@
         <v>1440.92</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>8173.64</v>
+        <v>11022.08</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>-6732.72</v>
+        <v>-9581.16</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>5.672514782222469</v>
+        <v>7.649335146989423</v>
       </c>
     </row>
     <row r="12">
@@ -6130,13 +6130,13 @@
         <v>57887.35196497848</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>37283.29</v>
+        <v>41556.97</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>20604.06196497848</v>
+        <v>16330.38196497848</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.6440662551390531</v>
+        <v>0.7178937814454137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2026-01-07 11:30:09
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -3365,13 +3365,13 @@
         <v>0</v>
       </c>
       <c r="M48" s="2" t="n">
-        <v>0</v>
+        <v>50.24</v>
       </c>
       <c r="N48" s="2" t="n">
         <v>0</v>
       </c>
       <c r="O48" s="2" t="n">
-        <v>0</v>
+        <v>3704.28</v>
       </c>
       <c r="P48" s="2" t="n">
         <v>0</v>
@@ -4156,17 +4156,17 @@
       </c>
       <c r="M61" s="4" t="inlineStr">
         <is>
+          <t>3 de 59</t>
+        </is>
+      </c>
+      <c r="N61" s="4" t="inlineStr">
+        <is>
+          <t>0 de 59</t>
+        </is>
+      </c>
+      <c r="O61" s="4" t="inlineStr">
+        <is>
           <t>2 de 59</t>
-        </is>
-      </c>
-      <c r="N61" s="4" t="inlineStr">
-        <is>
-          <t>0 de 59</t>
-        </is>
-      </c>
-      <c r="O61" s="4" t="inlineStr">
-        <is>
-          <t>1 de 59</t>
         </is>
       </c>
       <c r="P61" s="4" t="inlineStr">
@@ -5513,7 +5513,7 @@
         <v>8877.290000000001</v>
       </c>
       <c r="F48" s="2" t="n">
-        <v>0</v>
+        <v>3754.52</v>
       </c>
       <c r="G48" s="2" t="n">
         <v>2000</v>
@@ -5854,7 +5854,7 @@
         <v>57559.06</v>
       </c>
       <c r="F61" s="6" t="n">
-        <v>6142.42</v>
+        <v>9896.940000000001</v>
       </c>
       <c r="G61" s="6" t="n">
         <v>48000</v>

</xml_diff>

<commit_message>
Actualización automática 2026-01-07 15:30:08
</commit_message>
<xml_diff>
--- a/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
+++ b/data/LINDAO ZUÑIGA BRYAN JOSE.xlsx
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="2" t="n">
-        <v>0</v>
+        <v>1496.72</v>
       </c>
       <c r="N31" s="2" t="n">
         <v>0</v>
@@ -4156,7 +4156,7 @@
       </c>
       <c r="M61" s="4" t="inlineStr">
         <is>
-          <t>3 de 59</t>
+          <t>4 de 59</t>
         </is>
       </c>
       <c r="N61" s="4" t="inlineStr">
@@ -5054,7 +5054,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="2" t="n">
-        <v>0</v>
+        <v>1496.72</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>0</v>
@@ -5854,7 +5854,7 @@
         <v>57559.06</v>
       </c>
       <c r="F61" s="6" t="n">
-        <v>9896.940000000001</v>
+        <v>11393.66</v>
       </c>
       <c r="G61" s="6" t="n">
         <v>48000</v>

</xml_diff>